<commit_message>
bug fixing, need to sort out saving annotated plots
</commit_message>
<xml_diff>
--- a/myfile.xlsx
+++ b/myfile.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\coronavirus\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A043E68-C580-47AD-9DA2-C00472F8A19C}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6AA0C07-5B56-4784-AA2A-F3395B41CD8B}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1812" yWindow="1812" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1812" yWindow="1812" windowWidth="17280" windowHeight="8964" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="cases" sheetId="5" r:id="rId1"/>
@@ -2157,8 +2157,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:DA118"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A68" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E93" sqref="E93"/>
+    <sheetView topLeftCell="A68" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B91" sqref="B91"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -18199,7 +18199,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1F0720B9-F1C1-4E88-8345-0A7B8577FCEF}">
   <dimension ref="A1:CS82"/>
   <sheetViews>
-    <sheetView topLeftCell="CM74" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A74" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="CU82" sqref="CU82"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
daily email sent out
</commit_message>
<xml_diff>
--- a/myfile.xlsx
+++ b/myfile.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\coronavirus\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F8CEC96-00BC-4041-986A-40F7F6B84CC6}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A41110E0-9EDE-4E20-9E60-F85D62AF6D94}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1812" yWindow="1812" windowWidth="17280" windowHeight="8964" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="cases" sheetId="5" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1077" uniqueCount="379">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1087" uniqueCount="384">
   <si>
     <t>China</t>
   </si>
@@ -1168,6 +1168,21 @@
   </si>
   <si>
     <t>20.4.11</t>
+  </si>
+  <si>
+    <t>20.4.12</t>
+  </si>
+  <si>
+    <t>20.4.13</t>
+  </si>
+  <si>
+    <t>20.4.14</t>
+  </si>
+  <si>
+    <t>20.4.15</t>
+  </si>
+  <si>
+    <t>20.4.16</t>
   </si>
 </sst>
 </file>
@@ -1802,11 +1817,11 @@
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="42" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" textRotation="255" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="42" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" textRotation="255" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -2169,8 +2184,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:DA118"/>
   <sheetViews>
-    <sheetView topLeftCell="CQ79" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="CI96" sqref="CI96"/>
+    <sheetView topLeftCell="CF88" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="CJ101" sqref="CJ101"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2179,144 +2194,144 @@
       <c r="A1" s="3" t="s">
         <v>114</v>
       </c>
-      <c r="B1" s="24" t="s">
+      <c r="B1" s="25" t="s">
         <v>116</v>
       </c>
-      <c r="C1" s="24"/>
-      <c r="D1" s="24"/>
-      <c r="E1" s="24"/>
-      <c r="F1" s="24"/>
-      <c r="G1" s="24"/>
-      <c r="H1" s="24"/>
-      <c r="I1" s="24"/>
-      <c r="J1" s="24"/>
-      <c r="K1" s="24"/>
-      <c r="L1" s="24"/>
-      <c r="M1" s="24"/>
-      <c r="N1" s="24"/>
-      <c r="O1" s="24" t="s">
+      <c r="C1" s="25"/>
+      <c r="D1" s="25"/>
+      <c r="E1" s="25"/>
+      <c r="F1" s="25"/>
+      <c r="G1" s="25"/>
+      <c r="H1" s="25"/>
+      <c r="I1" s="25"/>
+      <c r="J1" s="25"/>
+      <c r="K1" s="25"/>
+      <c r="L1" s="25"/>
+      <c r="M1" s="25"/>
+      <c r="N1" s="25"/>
+      <c r="O1" s="25" t="s">
         <v>117</v>
       </c>
-      <c r="P1" s="24"/>
+      <c r="P1" s="25"/>
       <c r="Q1" s="3" t="s">
         <v>118</v>
       </c>
-      <c r="R1" s="24" t="s">
+      <c r="R1" s="25" t="s">
         <v>119</v>
       </c>
-      <c r="S1" s="24"/>
-      <c r="T1" s="24" t="s">
+      <c r="S1" s="25"/>
+      <c r="T1" s="25" t="s">
         <v>120</v>
       </c>
-      <c r="U1" s="24"/>
-      <c r="V1" s="24"/>
-      <c r="W1" s="24"/>
-      <c r="X1" s="24" t="s">
+      <c r="U1" s="25"/>
+      <c r="V1" s="25"/>
+      <c r="W1" s="25"/>
+      <c r="X1" s="25" t="s">
         <v>121</v>
       </c>
-      <c r="Y1" s="24"/>
+      <c r="Y1" s="25"/>
       <c r="Z1" s="3" t="s">
         <v>122</v>
       </c>
       <c r="AA1" s="3" t="s">
         <v>114</v>
       </c>
-      <c r="AB1" s="24" t="s">
+      <c r="AB1" s="25" t="s">
         <v>123</v>
       </c>
-      <c r="AC1" s="24"/>
-      <c r="AD1" s="24"/>
-      <c r="AE1" s="24"/>
-      <c r="AF1" s="24"/>
-      <c r="AG1" s="24" t="s">
+      <c r="AC1" s="25"/>
+      <c r="AD1" s="25"/>
+      <c r="AE1" s="25"/>
+      <c r="AF1" s="25"/>
+      <c r="AG1" s="25" t="s">
         <v>124</v>
       </c>
-      <c r="AH1" s="24"/>
-      <c r="AI1" s="24"/>
-      <c r="AJ1" s="24"/>
-      <c r="AK1" s="24"/>
-      <c r="AL1" s="24"/>
-      <c r="AM1" s="24"/>
-      <c r="AN1" s="24"/>
-      <c r="AO1" s="24"/>
-      <c r="AP1" s="24"/>
-      <c r="AQ1" s="24"/>
-      <c r="AR1" s="24" t="s">
+      <c r="AH1" s="25"/>
+      <c r="AI1" s="25"/>
+      <c r="AJ1" s="25"/>
+      <c r="AK1" s="25"/>
+      <c r="AL1" s="25"/>
+      <c r="AM1" s="25"/>
+      <c r="AN1" s="25"/>
+      <c r="AO1" s="25"/>
+      <c r="AP1" s="25"/>
+      <c r="AQ1" s="25"/>
+      <c r="AR1" s="25" t="s">
         <v>125</v>
       </c>
-      <c r="AS1" s="24"/>
-      <c r="AT1" s="24" t="s">
+      <c r="AS1" s="25"/>
+      <c r="AT1" s="25" t="s">
         <v>126</v>
       </c>
-      <c r="AU1" s="24"/>
-      <c r="AV1" s="24"/>
-      <c r="AW1" s="24"/>
-      <c r="AX1" s="24"/>
-      <c r="AY1" s="24" t="s">
+      <c r="AU1" s="25"/>
+      <c r="AV1" s="25"/>
+      <c r="AW1" s="25"/>
+      <c r="AX1" s="25"/>
+      <c r="AY1" s="25" t="s">
         <v>127</v>
       </c>
-      <c r="AZ1" s="24"/>
-      <c r="BA1" s="24"/>
-      <c r="BB1" s="24"/>
-      <c r="BC1" s="24"/>
-      <c r="BD1" s="24"/>
-      <c r="BE1" s="24"/>
-      <c r="BF1" s="24"/>
-      <c r="BG1" s="24"/>
-      <c r="BH1" s="24"/>
-      <c r="BI1" s="24"/>
-      <c r="BJ1" s="24"/>
-      <c r="BK1" s="24"/>
-      <c r="BL1" s="24"/>
+      <c r="AZ1" s="25"/>
+      <c r="BA1" s="25"/>
+      <c r="BB1" s="25"/>
+      <c r="BC1" s="25"/>
+      <c r="BD1" s="25"/>
+      <c r="BE1" s="25"/>
+      <c r="BF1" s="25"/>
+      <c r="BG1" s="25"/>
+      <c r="BH1" s="25"/>
+      <c r="BI1" s="25"/>
+      <c r="BJ1" s="25"/>
+      <c r="BK1" s="25"/>
+      <c r="BL1" s="25"/>
       <c r="BM1" s="3" t="s">
         <v>114</v>
       </c>
-      <c r="BN1" s="24" t="s">
+      <c r="BN1" s="25" t="s">
         <v>128</v>
       </c>
-      <c r="BO1" s="24"/>
-      <c r="BP1" s="24"/>
-      <c r="BQ1" s="24"/>
-      <c r="BR1" s="24"/>
-      <c r="BS1" s="24"/>
-      <c r="BT1" s="24"/>
-      <c r="BU1" s="24"/>
-      <c r="BV1" s="24"/>
-      <c r="BW1" s="24"/>
-      <c r="BX1" s="24"/>
-      <c r="BY1" s="24" t="s">
+      <c r="BO1" s="25"/>
+      <c r="BP1" s="25"/>
+      <c r="BQ1" s="25"/>
+      <c r="BR1" s="25"/>
+      <c r="BS1" s="25"/>
+      <c r="BT1" s="25"/>
+      <c r="BU1" s="25"/>
+      <c r="BV1" s="25"/>
+      <c r="BW1" s="25"/>
+      <c r="BX1" s="25"/>
+      <c r="BY1" s="25" t="s">
         <v>129</v>
       </c>
-      <c r="BZ1" s="24"/>
-      <c r="CA1" s="24"/>
-      <c r="CB1" s="24"/>
-      <c r="CC1" s="24"/>
-      <c r="CD1" s="24"/>
-      <c r="CE1" s="24"/>
-      <c r="CF1" s="24"/>
-      <c r="CG1" s="24"/>
-      <c r="CH1" s="24" t="s">
+      <c r="BZ1" s="25"/>
+      <c r="CA1" s="25"/>
+      <c r="CB1" s="25"/>
+      <c r="CC1" s="25"/>
+      <c r="CD1" s="25"/>
+      <c r="CE1" s="25"/>
+      <c r="CF1" s="25"/>
+      <c r="CG1" s="25"/>
+      <c r="CH1" s="25" t="s">
         <v>130</v>
       </c>
-      <c r="CI1" s="24"/>
-      <c r="CJ1" s="24"/>
-      <c r="CK1" s="24"/>
-      <c r="CL1" s="24"/>
-      <c r="CM1" s="24"/>
-      <c r="CN1" s="24"/>
-      <c r="CO1" s="24"/>
-      <c r="CP1" s="24"/>
-      <c r="CQ1" s="24"/>
-      <c r="CR1" s="24" t="s">
+      <c r="CI1" s="25"/>
+      <c r="CJ1" s="25"/>
+      <c r="CK1" s="25"/>
+      <c r="CL1" s="25"/>
+      <c r="CM1" s="25"/>
+      <c r="CN1" s="25"/>
+      <c r="CO1" s="25"/>
+      <c r="CP1" s="25"/>
+      <c r="CQ1" s="25"/>
+      <c r="CR1" s="25" t="s">
         <v>131</v>
       </c>
-      <c r="CS1" s="24"/>
-      <c r="CT1" s="24"/>
-      <c r="CU1" s="24"/>
-      <c r="CV1" s="24"/>
-      <c r="CW1" s="24"/>
-      <c r="CX1" s="24"/>
-      <c r="CY1" s="24"/>
+      <c r="CS1" s="25"/>
+      <c r="CT1" s="25"/>
+      <c r="CU1" s="25"/>
+      <c r="CV1" s="25"/>
+      <c r="CW1" s="25"/>
+      <c r="CX1" s="25"/>
+      <c r="CY1" s="25"/>
       <c r="CZ1" s="3" t="s">
         <v>361</v>
       </c>
@@ -2325,43 +2340,43 @@
       <c r="A2" s="3" t="s">
         <v>115</v>
       </c>
-      <c r="B2" s="25" t="s">
+      <c r="B2" s="24" t="s">
         <v>41</v>
       </c>
-      <c r="C2" s="25" t="s">
+      <c r="C2" s="24" t="s">
         <v>24</v>
       </c>
-      <c r="D2" s="25" t="s">
+      <c r="D2" s="24" t="s">
         <v>22</v>
       </c>
-      <c r="E2" s="25" t="s">
+      <c r="E2" s="24" t="s">
         <v>16</v>
       </c>
-      <c r="F2" s="25" t="s">
+      <c r="F2" s="24" t="s">
         <v>43</v>
       </c>
-      <c r="G2" s="25" t="s">
+      <c r="G2" s="24" t="s">
         <v>49</v>
       </c>
-      <c r="H2" s="25" t="s">
+      <c r="H2" s="24" t="s">
         <v>64</v>
       </c>
-      <c r="I2" s="25" t="s">
+      <c r="I2" s="24" t="s">
         <v>84</v>
       </c>
-      <c r="J2" s="25" t="s">
+      <c r="J2" s="24" t="s">
         <v>95</v>
       </c>
-      <c r="K2" s="25" t="s">
+      <c r="K2" s="24" t="s">
         <v>97</v>
       </c>
-      <c r="L2" s="25" t="s">
+      <c r="L2" s="24" t="s">
         <v>101</v>
       </c>
-      <c r="M2" s="25" t="s">
+      <c r="M2" s="24" t="s">
         <v>108</v>
       </c>
-      <c r="N2" s="25" t="s">
+      <c r="N2" s="24" t="s">
         <v>105</v>
       </c>
       <c r="O2" s="4" t="s">
@@ -2370,148 +2385,148 @@
       <c r="P2" s="4" t="s">
         <v>134</v>
       </c>
-      <c r="Q2" s="25" t="s">
+      <c r="Q2" s="24" t="s">
         <v>42</v>
       </c>
-      <c r="R2" s="25" t="s">
+      <c r="R2" s="24" t="s">
         <v>368</v>
       </c>
-      <c r="S2" s="25" t="s">
+      <c r="S2" s="24" t="s">
         <v>10</v>
       </c>
-      <c r="T2" s="25" t="s">
+      <c r="T2" s="24" t="s">
         <v>48</v>
       </c>
-      <c r="U2" s="25" t="s">
+      <c r="U2" s="24" t="s">
         <v>56</v>
       </c>
-      <c r="V2" s="25" t="s">
+      <c r="V2" s="24" t="s">
         <v>67</v>
       </c>
-      <c r="W2" s="25" t="s">
+      <c r="W2" s="24" t="s">
         <v>62</v>
       </c>
-      <c r="X2" s="25" t="s">
+      <c r="X2" s="24" t="s">
         <v>94</v>
       </c>
-      <c r="Y2" s="25" t="s">
+      <c r="Y2" s="24" t="s">
         <v>82</v>
       </c>
-      <c r="Z2" s="25" t="s">
+      <c r="Z2" s="24" t="s">
         <v>33</v>
       </c>
       <c r="AA2" s="3" t="s">
         <v>115</v>
       </c>
-      <c r="AB2" s="25" t="s">
+      <c r="AB2" s="24" t="s">
         <v>47</v>
       </c>
-      <c r="AC2" s="25" t="s">
+      <c r="AC2" s="24" t="s">
         <v>137</v>
       </c>
-      <c r="AD2" s="25" t="s">
+      <c r="AD2" s="24" t="s">
         <v>63</v>
       </c>
-      <c r="AE2" s="25" t="s">
+      <c r="AE2" s="24" t="s">
         <v>138</v>
       </c>
-      <c r="AF2" s="25" t="s">
+      <c r="AF2" s="24" t="s">
         <v>23</v>
       </c>
-      <c r="AG2" s="25" t="s">
+      <c r="AG2" s="24" t="s">
         <v>76</v>
       </c>
-      <c r="AH2" s="25" t="s">
+      <c r="AH2" s="24" t="s">
         <v>86</v>
       </c>
-      <c r="AI2" s="25" t="s">
+      <c r="AI2" s="24" t="s">
         <v>28</v>
       </c>
-      <c r="AJ2" s="25" t="s">
+      <c r="AJ2" s="24" t="s">
         <v>18</v>
       </c>
-      <c r="AK2" s="25" t="s">
+      <c r="AK2" s="24" t="s">
         <v>38</v>
       </c>
-      <c r="AL2" s="25" t="s">
+      <c r="AL2" s="24" t="s">
         <v>35</v>
       </c>
-      <c r="AM2" s="25" t="s">
+      <c r="AM2" s="24" t="s">
         <v>29</v>
       </c>
-      <c r="AN2" s="25" t="s">
+      <c r="AN2" s="24" t="s">
         <v>83</v>
       </c>
-      <c r="AO2" s="25" t="s">
+      <c r="AO2" s="24" t="s">
         <v>342</v>
       </c>
-      <c r="AP2" s="25" t="s">
+      <c r="AP2" s="24" t="s">
         <v>107</v>
       </c>
-      <c r="AQ2" s="25" t="s">
+      <c r="AQ2" s="24" t="s">
         <v>110</v>
       </c>
-      <c r="AR2" s="25" t="s">
+      <c r="AR2" s="24" t="s">
         <v>14</v>
       </c>
-      <c r="AS2" s="25" t="s">
+      <c r="AS2" s="24" t="s">
         <v>55</v>
       </c>
-      <c r="AT2" s="25" t="s">
+      <c r="AT2" s="24" t="s">
         <v>113</v>
       </c>
-      <c r="AU2" s="25" t="s">
+      <c r="AU2" s="24" t="s">
         <v>37</v>
       </c>
-      <c r="AV2" s="25" t="s">
+      <c r="AV2" s="24" t="s">
         <v>26</v>
       </c>
-      <c r="AW2" s="25" t="s">
+      <c r="AW2" s="24" t="s">
         <v>85</v>
       </c>
-      <c r="AX2" s="25" t="s">
+      <c r="AX2" s="24" t="s">
         <v>87</v>
       </c>
-      <c r="AY2" s="25" t="s">
+      <c r="AY2" s="24" t="s">
         <v>72</v>
       </c>
-      <c r="AZ2" s="25" t="s">
+      <c r="AZ2" s="24" t="s">
         <v>32</v>
       </c>
-      <c r="BA2" s="25" t="s">
+      <c r="BA2" s="24" t="s">
         <v>69</v>
       </c>
-      <c r="BB2" s="25" t="s">
+      <c r="BB2" s="24" t="s">
         <v>46</v>
       </c>
-      <c r="BC2" s="25" t="s">
+      <c r="BC2" s="24" t="s">
         <v>80</v>
       </c>
-      <c r="BD2" s="25" t="s">
+      <c r="BD2" s="24" t="s">
         <v>51</v>
       </c>
       <c r="BE2" s="4" t="s">
         <v>139</v>
       </c>
-      <c r="BF2" s="25" t="s">
+      <c r="BF2" s="24" t="s">
         <v>4</v>
       </c>
-      <c r="BG2" s="25" t="s">
+      <c r="BG2" s="24" t="s">
         <v>52</v>
       </c>
-      <c r="BH2" s="25" t="s">
+      <c r="BH2" s="24" t="s">
         <v>81</v>
       </c>
-      <c r="BI2" s="25" t="s">
+      <c r="BI2" s="24" t="s">
         <v>58</v>
       </c>
-      <c r="BJ2" s="25" t="s">
+      <c r="BJ2" s="24" t="s">
         <v>91</v>
       </c>
-      <c r="BK2" s="25" t="s">
+      <c r="BK2" s="24" t="s">
         <v>54</v>
       </c>
-      <c r="BL2" s="25" t="s">
+      <c r="BL2" s="24" t="s">
         <v>15</v>
       </c>
       <c r="BM2" s="3" t="s">
@@ -2520,115 +2535,115 @@
       <c r="BN2" s="4" t="s">
         <v>141</v>
       </c>
-      <c r="BO2" s="25" t="s">
+      <c r="BO2" s="24" t="s">
         <v>34</v>
       </c>
       <c r="BP2" s="4" t="s">
         <v>143</v>
       </c>
-      <c r="BQ2" s="25" t="s">
+      <c r="BQ2" s="24" t="s">
         <v>45</v>
       </c>
-      <c r="BR2" s="25" t="s">
+      <c r="BR2" s="24" t="s">
         <v>73</v>
       </c>
-      <c r="BS2" s="25" t="s">
-        <v>1</v>
-      </c>
-      <c r="BT2" s="25" t="s">
+      <c r="BS2" s="24" t="s">
+        <v>1</v>
+      </c>
+      <c r="BT2" s="24" t="s">
         <v>99</v>
       </c>
-      <c r="BU2" s="25" t="s">
+      <c r="BU2" s="24" t="s">
         <v>12</v>
       </c>
-      <c r="BV2" s="25" t="s">
+      <c r="BV2" s="24" t="s">
         <v>40</v>
       </c>
-      <c r="BW2" s="25" t="s">
+      <c r="BW2" s="24" t="s">
         <v>2</v>
       </c>
-      <c r="BX2" s="25" t="s">
+      <c r="BX2" s="24" t="s">
         <v>70</v>
       </c>
-      <c r="BY2" s="25" t="s">
+      <c r="BY2" s="24" t="s">
         <v>5</v>
       </c>
-      <c r="BZ2" s="25" t="s">
+      <c r="BZ2" s="24" t="s">
         <v>100</v>
       </c>
-      <c r="CA2" s="25" t="s">
+      <c r="CA2" s="24" t="s">
         <v>6</v>
       </c>
-      <c r="CB2" s="25" t="s">
+      <c r="CB2" s="24" t="s">
         <v>8</v>
       </c>
-      <c r="CC2" s="25" t="s">
+      <c r="CC2" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="CD2" s="25" t="s">
+      <c r="CD2" s="24" t="s">
         <v>21</v>
       </c>
-      <c r="CE2" s="25" t="s">
+      <c r="CE2" s="24" t="s">
         <v>96</v>
       </c>
-      <c r="CF2" s="25" t="s">
+      <c r="CF2" s="24" t="s">
         <v>9</v>
       </c>
-      <c r="CG2" s="25" t="s">
+      <c r="CG2" s="24" t="s">
         <v>7</v>
       </c>
       <c r="CH2" s="4" t="s">
         <v>369</v>
       </c>
-      <c r="CI2" s="25" t="s">
+      <c r="CI2" s="24" t="s">
         <v>20</v>
       </c>
-      <c r="CJ2" s="25" t="s">
+      <c r="CJ2" s="24" t="s">
         <v>36</v>
       </c>
-      <c r="CK2" s="25" t="s">
+      <c r="CK2" s="24" t="s">
         <v>13</v>
       </c>
-      <c r="CL2" s="25" t="s">
+      <c r="CL2" s="24" t="s">
         <v>19</v>
       </c>
-      <c r="CM2" s="25" t="s">
+      <c r="CM2" s="24" t="s">
         <v>17</v>
       </c>
-      <c r="CN2" s="25" t="s">
+      <c r="CN2" s="24" t="s">
         <v>30</v>
       </c>
-      <c r="CO2" s="25" t="s">
+      <c r="CO2" s="24" t="s">
         <v>44</v>
       </c>
-      <c r="CP2" s="25" t="s">
+      <c r="CP2" s="24" t="s">
         <v>60</v>
       </c>
-      <c r="CQ2" s="25" t="s">
+      <c r="CQ2" s="24" t="s">
         <v>57</v>
       </c>
-      <c r="CR2" s="25" t="s">
+      <c r="CR2" s="24" t="s">
         <v>27</v>
       </c>
       <c r="CS2" s="4" t="s">
         <v>146</v>
       </c>
-      <c r="CT2" s="25" t="s">
+      <c r="CT2" s="24" t="s">
         <v>59</v>
       </c>
-      <c r="CU2" s="25" t="s">
+      <c r="CU2" s="24" t="s">
         <v>25</v>
       </c>
-      <c r="CV2" s="25" t="s">
+      <c r="CV2" s="24" t="s">
         <v>88</v>
       </c>
-      <c r="CW2" s="25" t="s">
+      <c r="CW2" s="24" t="s">
         <v>68</v>
       </c>
       <c r="CX2" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="CY2" s="25" t="s">
+      <c r="CY2" s="24" t="s">
         <v>31</v>
       </c>
       <c r="CZ2" s="5" t="s">
@@ -2640,122 +2655,122 @@
     </row>
     <row r="3" spans="1:105" ht="87.6" x14ac:dyDescent="0.3">
       <c r="A3" s="3"/>
-      <c r="B3" s="25"/>
-      <c r="C3" s="25"/>
-      <c r="D3" s="25"/>
-      <c r="E3" s="25"/>
-      <c r="F3" s="25"/>
-      <c r="G3" s="25"/>
-      <c r="H3" s="25"/>
-      <c r="I3" s="25"/>
-      <c r="J3" s="25"/>
-      <c r="K3" s="25"/>
-      <c r="L3" s="25"/>
-      <c r="M3" s="25"/>
-      <c r="N3" s="25"/>
+      <c r="B3" s="24"/>
+      <c r="C3" s="24"/>
+      <c r="D3" s="24"/>
+      <c r="E3" s="24"/>
+      <c r="F3" s="24"/>
+      <c r="G3" s="24"/>
+      <c r="H3" s="24"/>
+      <c r="I3" s="24"/>
+      <c r="J3" s="24"/>
+      <c r="K3" s="24"/>
+      <c r="L3" s="24"/>
+      <c r="M3" s="24"/>
+      <c r="N3" s="24"/>
       <c r="O3" s="4" t="s">
         <v>133</v>
       </c>
       <c r="P3" s="4" t="s">
         <v>135</v>
       </c>
-      <c r="Q3" s="25"/>
-      <c r="R3" s="25"/>
-      <c r="S3" s="25"/>
-      <c r="T3" s="25"/>
-      <c r="U3" s="25"/>
-      <c r="V3" s="25"/>
-      <c r="W3" s="25"/>
-      <c r="X3" s="25"/>
-      <c r="Y3" s="25"/>
-      <c r="Z3" s="25"/>
+      <c r="Q3" s="24"/>
+      <c r="R3" s="24"/>
+      <c r="S3" s="24"/>
+      <c r="T3" s="24"/>
+      <c r="U3" s="24"/>
+      <c r="V3" s="24"/>
+      <c r="W3" s="24"/>
+      <c r="X3" s="24"/>
+      <c r="Y3" s="24"/>
+      <c r="Z3" s="24"/>
       <c r="AA3" s="3"/>
-      <c r="AB3" s="25"/>
-      <c r="AC3" s="25"/>
-      <c r="AD3" s="25"/>
-      <c r="AE3" s="25"/>
-      <c r="AF3" s="25"/>
-      <c r="AG3" s="25"/>
-      <c r="AH3" s="25"/>
-      <c r="AI3" s="25"/>
-      <c r="AJ3" s="25"/>
-      <c r="AK3" s="25"/>
-      <c r="AL3" s="25"/>
-      <c r="AM3" s="25"/>
-      <c r="AN3" s="25"/>
-      <c r="AO3" s="25"/>
-      <c r="AP3" s="25"/>
-      <c r="AQ3" s="25"/>
-      <c r="AR3" s="25"/>
-      <c r="AS3" s="25"/>
-      <c r="AT3" s="25"/>
-      <c r="AU3" s="25"/>
-      <c r="AV3" s="25"/>
-      <c r="AW3" s="25"/>
-      <c r="AX3" s="25"/>
-      <c r="AY3" s="25"/>
-      <c r="AZ3" s="25"/>
-      <c r="BA3" s="25"/>
-      <c r="BB3" s="25"/>
-      <c r="BC3" s="25"/>
-      <c r="BD3" s="25"/>
+      <c r="AB3" s="24"/>
+      <c r="AC3" s="24"/>
+      <c r="AD3" s="24"/>
+      <c r="AE3" s="24"/>
+      <c r="AF3" s="24"/>
+      <c r="AG3" s="24"/>
+      <c r="AH3" s="24"/>
+      <c r="AI3" s="24"/>
+      <c r="AJ3" s="24"/>
+      <c r="AK3" s="24"/>
+      <c r="AL3" s="24"/>
+      <c r="AM3" s="24"/>
+      <c r="AN3" s="24"/>
+      <c r="AO3" s="24"/>
+      <c r="AP3" s="24"/>
+      <c r="AQ3" s="24"/>
+      <c r="AR3" s="24"/>
+      <c r="AS3" s="24"/>
+      <c r="AT3" s="24"/>
+      <c r="AU3" s="24"/>
+      <c r="AV3" s="24"/>
+      <c r="AW3" s="24"/>
+      <c r="AX3" s="24"/>
+      <c r="AY3" s="24"/>
+      <c r="AZ3" s="24"/>
+      <c r="BA3" s="24"/>
+      <c r="BB3" s="24"/>
+      <c r="BC3" s="24"/>
+      <c r="BD3" s="24"/>
       <c r="BE3" s="4" t="s">
         <v>140</v>
       </c>
-      <c r="BF3" s="25"/>
-      <c r="BG3" s="25"/>
-      <c r="BH3" s="25"/>
-      <c r="BI3" s="25"/>
-      <c r="BJ3" s="25"/>
-      <c r="BK3" s="25"/>
-      <c r="BL3" s="25"/>
+      <c r="BF3" s="24"/>
+      <c r="BG3" s="24"/>
+      <c r="BH3" s="24"/>
+      <c r="BI3" s="24"/>
+      <c r="BJ3" s="24"/>
+      <c r="BK3" s="24"/>
+      <c r="BL3" s="24"/>
       <c r="BM3" s="3"/>
       <c r="BN3" s="4" t="s">
         <v>142</v>
       </c>
-      <c r="BO3" s="25"/>
+      <c r="BO3" s="24"/>
       <c r="BP3" s="4" t="s">
         <v>144</v>
       </c>
-      <c r="BQ3" s="25"/>
-      <c r="BR3" s="25"/>
-      <c r="BS3" s="25"/>
-      <c r="BT3" s="25"/>
-      <c r="BU3" s="25"/>
-      <c r="BV3" s="25"/>
-      <c r="BW3" s="25"/>
-      <c r="BX3" s="25"/>
-      <c r="BY3" s="25"/>
-      <c r="BZ3" s="25"/>
-      <c r="CA3" s="25"/>
-      <c r="CB3" s="25"/>
-      <c r="CC3" s="25"/>
-      <c r="CD3" s="25"/>
-      <c r="CE3" s="25"/>
-      <c r="CF3" s="25"/>
-      <c r="CG3" s="25"/>
+      <c r="BQ3" s="24"/>
+      <c r="BR3" s="24"/>
+      <c r="BS3" s="24"/>
+      <c r="BT3" s="24"/>
+      <c r="BU3" s="24"/>
+      <c r="BV3" s="24"/>
+      <c r="BW3" s="24"/>
+      <c r="BX3" s="24"/>
+      <c r="BY3" s="24"/>
+      <c r="BZ3" s="24"/>
+      <c r="CA3" s="24"/>
+      <c r="CB3" s="24"/>
+      <c r="CC3" s="24"/>
+      <c r="CD3" s="24"/>
+      <c r="CE3" s="24"/>
+      <c r="CF3" s="24"/>
+      <c r="CG3" s="24"/>
       <c r="CH3" s="4" t="s">
         <v>145</v>
       </c>
-      <c r="CI3" s="25"/>
-      <c r="CJ3" s="25"/>
-      <c r="CK3" s="25"/>
-      <c r="CL3" s="25"/>
-      <c r="CM3" s="25"/>
-      <c r="CN3" s="25"/>
-      <c r="CO3" s="25"/>
-      <c r="CP3" s="25"/>
-      <c r="CQ3" s="25"/>
-      <c r="CR3" s="25"/>
+      <c r="CI3" s="24"/>
+      <c r="CJ3" s="24"/>
+      <c r="CK3" s="24"/>
+      <c r="CL3" s="24"/>
+      <c r="CM3" s="24"/>
+      <c r="CN3" s="24"/>
+      <c r="CO3" s="24"/>
+      <c r="CP3" s="24"/>
+      <c r="CQ3" s="24"/>
+      <c r="CR3" s="24"/>
       <c r="CS3" s="4" t="s">
         <v>133</v>
       </c>
-      <c r="CT3" s="25"/>
-      <c r="CU3" s="25"/>
-      <c r="CV3" s="25"/>
-      <c r="CW3" s="25"/>
+      <c r="CT3" s="24"/>
+      <c r="CU3" s="24"/>
+      <c r="CV3" s="24"/>
+      <c r="CW3" s="24"/>
       <c r="CX3" s="14"/>
-      <c r="CY3" s="25"/>
+      <c r="CY3" s="24"/>
       <c r="CZ3" s="5"/>
     </row>
     <row r="4" spans="1:105" ht="15.6" x14ac:dyDescent="0.3">
@@ -17582,6 +17597,9 @@
       <c r="BY94" s="2">
         <v>4799</v>
       </c>
+      <c r="CC94" s="2">
+        <v>4939</v>
+      </c>
       <c r="CD94" s="2"/>
       <c r="CH94" s="2">
         <v>4344</v>
@@ -17604,6 +17622,9 @@
       <c r="BY95" s="2">
         <v>7120</v>
       </c>
+      <c r="CC95" s="2">
+        <v>3936</v>
+      </c>
       <c r="CD95" s="2"/>
       <c r="CH95" s="2">
         <v>8681</v>
@@ -17626,71 +17647,176 @@
       <c r="BY96" s="2">
         <v>4785</v>
       </c>
+      <c r="CC96" s="2">
+        <v>3281</v>
+      </c>
       <c r="CD96" s="2"/>
       <c r="CH96" s="2">
         <v>5233</v>
       </c>
     </row>
-    <row r="97" spans="1:82" x14ac:dyDescent="0.3">
-      <c r="A97" s="2"/>
+    <row r="97" spans="1:86" x14ac:dyDescent="0.3">
+      <c r="A97" s="2" t="s">
+        <v>379</v>
+      </c>
+      <c r="R97" s="2">
+        <v>27421</v>
+      </c>
       <c r="BM97" s="2"/>
+      <c r="BS97" s="2">
+        <v>4092</v>
+      </c>
+      <c r="BW97" s="2">
+        <v>3804</v>
+      </c>
+      <c r="BY97" s="2">
+        <v>2937</v>
+      </c>
+      <c r="CC97" s="2">
+        <v>2402</v>
+      </c>
       <c r="CD97" s="2"/>
+      <c r="CH97" s="2">
+        <v>5288</v>
+      </c>
     </row>
-    <row r="98" spans="1:82" x14ac:dyDescent="0.3">
-      <c r="A98" s="2"/>
+    <row r="98" spans="1:86" x14ac:dyDescent="0.3">
+      <c r="A98" s="2" t="s">
+        <v>380</v>
+      </c>
+      <c r="R98" s="2">
+        <v>26641</v>
+      </c>
       <c r="BM98" s="2"/>
+      <c r="BS98" s="2">
+        <v>3153</v>
+      </c>
+      <c r="BW98" s="2">
+        <v>3268</v>
+      </c>
+      <c r="BY98" s="2">
+        <v>4188</v>
+      </c>
+      <c r="CC98" s="2">
+        <v>2218</v>
+      </c>
       <c r="CD98" s="2"/>
+      <c r="CH98" s="2">
+        <v>4342</v>
+      </c>
     </row>
-    <row r="99" spans="1:82" x14ac:dyDescent="0.3">
-      <c r="A99" s="2"/>
+    <row r="99" spans="1:86" x14ac:dyDescent="0.3">
+      <c r="A99" s="2" t="s">
+        <v>381</v>
+      </c>
+      <c r="R99" s="2">
+        <v>30720</v>
+      </c>
       <c r="BM99" s="2"/>
+      <c r="BS99" s="2">
+        <v>2972</v>
+      </c>
+      <c r="BW99" s="2">
+        <v>3961</v>
+      </c>
+      <c r="BY99" s="2">
+        <v>6524</v>
+      </c>
+      <c r="CC99" s="2">
+        <v>2138</v>
+      </c>
       <c r="CD99" s="2"/>
+      <c r="CH99" s="2">
+        <v>5252</v>
+      </c>
     </row>
-    <row r="100" spans="1:82" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:86" x14ac:dyDescent="0.3">
+      <c r="A100" s="2" t="s">
+        <v>382</v>
+      </c>
+      <c r="R100" s="2">
+        <v>30342</v>
+      </c>
+      <c r="BS100" s="2">
+        <v>2667</v>
+      </c>
+      <c r="BW100" s="2">
+        <v>6599</v>
+      </c>
+      <c r="BY100" s="2">
+        <v>4560</v>
+      </c>
+      <c r="CC100" s="2">
+        <v>2543</v>
+      </c>
       <c r="CD100" s="2"/>
+      <c r="CH100" s="2">
+        <v>4603</v>
+      </c>
     </row>
-    <row r="101" spans="1:82" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:86" x14ac:dyDescent="0.3">
+      <c r="A101" s="2" t="s">
+        <v>383</v>
+      </c>
+      <c r="R101" s="2">
+        <v>29567</v>
+      </c>
+      <c r="BS101" s="2">
+        <v>3786</v>
+      </c>
+      <c r="BW101" s="2">
+        <v>4289</v>
+      </c>
+      <c r="BY101" s="2">
+        <v>17164</v>
+      </c>
+      <c r="CC101" s="2">
+        <v>2945</v>
+      </c>
       <c r="CD101" s="2"/>
+      <c r="CH101" s="2">
+        <v>4617</v>
+      </c>
     </row>
-    <row r="102" spans="1:82" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:86" x14ac:dyDescent="0.3">
       <c r="CD102" s="2"/>
     </row>
-    <row r="103" spans="1:82" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:86" x14ac:dyDescent="0.3">
       <c r="CD103" s="2"/>
     </row>
-    <row r="104" spans="1:82" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:86" x14ac:dyDescent="0.3">
       <c r="CC104" s="2"/>
       <c r="CD104" s="2"/>
     </row>
-    <row r="105" spans="1:82" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:86" x14ac:dyDescent="0.3">
       <c r="CC105" s="2"/>
       <c r="CD105" s="2"/>
     </row>
-    <row r="106" spans="1:82" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:86" x14ac:dyDescent="0.3">
       <c r="CC106" s="2"/>
       <c r="CD106" s="2"/>
     </row>
-    <row r="107" spans="1:82" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:86" x14ac:dyDescent="0.3">
       <c r="CC107" s="2"/>
       <c r="CD107" s="2"/>
     </row>
-    <row r="108" spans="1:82" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:86" x14ac:dyDescent="0.3">
       <c r="CC108" s="2"/>
       <c r="CD108" s="2"/>
     </row>
-    <row r="109" spans="1:82" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:86" x14ac:dyDescent="0.3">
       <c r="CC109" s="2"/>
       <c r="CD109" s="2"/>
     </row>
-    <row r="110" spans="1:82" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:86" x14ac:dyDescent="0.3">
       <c r="CC110" s="2"/>
       <c r="CD110" s="2"/>
     </row>
-    <row r="111" spans="1:82" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:86" x14ac:dyDescent="0.3">
       <c r="CC111" s="2"/>
       <c r="CD111" s="2"/>
     </row>
-    <row r="112" spans="1:82" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:86" x14ac:dyDescent="0.3">
       <c r="CC112" s="2"/>
       <c r="CD112" s="2"/>
     </row>
@@ -17714,64 +17840,30 @@
     </row>
   </sheetData>
   <mergeCells count="106">
-    <mergeCell ref="BV2:BV3"/>
-    <mergeCell ref="BW2:BW3"/>
-    <mergeCell ref="BX2:BX3"/>
-    <mergeCell ref="BY2:BY3"/>
-    <mergeCell ref="BO2:BO3"/>
-    <mergeCell ref="BQ2:BQ3"/>
-    <mergeCell ref="BR2:BR3"/>
-    <mergeCell ref="CN2:CN3"/>
-    <mergeCell ref="CG2:CG3"/>
-    <mergeCell ref="CI2:CI3"/>
-    <mergeCell ref="CJ2:CJ3"/>
-    <mergeCell ref="CK2:CK3"/>
-    <mergeCell ref="CM2:CM3"/>
-    <mergeCell ref="BZ2:BZ3"/>
-    <mergeCell ref="CA2:CA3"/>
-    <mergeCell ref="CB2:CB3"/>
-    <mergeCell ref="CC2:CC3"/>
-    <mergeCell ref="CD2:CD3"/>
-    <mergeCell ref="CE2:CE3"/>
-    <mergeCell ref="BS2:BS3"/>
-    <mergeCell ref="BT2:BT3"/>
-    <mergeCell ref="BG2:BG3"/>
-    <mergeCell ref="BH2:BH3"/>
-    <mergeCell ref="BI2:BI3"/>
-    <mergeCell ref="BJ2:BJ3"/>
-    <mergeCell ref="BK2:BK3"/>
-    <mergeCell ref="BL2:BL3"/>
-    <mergeCell ref="AX2:AX3"/>
-    <mergeCell ref="AY2:AY3"/>
-    <mergeCell ref="BB2:BB3"/>
-    <mergeCell ref="BD2:BD3"/>
-    <mergeCell ref="BF2:BF3"/>
-    <mergeCell ref="AQ2:AQ3"/>
-    <mergeCell ref="AS2:AS3"/>
-    <mergeCell ref="AT2:AT3"/>
-    <mergeCell ref="AU2:AU3"/>
-    <mergeCell ref="AV2:AV3"/>
-    <mergeCell ref="AW2:AW3"/>
-    <mergeCell ref="AK2:AK3"/>
-    <mergeCell ref="AL2:AL3"/>
-    <mergeCell ref="AM2:AM3"/>
-    <mergeCell ref="AN2:AN3"/>
-    <mergeCell ref="AO2:AO3"/>
-    <mergeCell ref="AP2:AP3"/>
-    <mergeCell ref="Q2:Q3"/>
-    <mergeCell ref="T1:W1"/>
-    <mergeCell ref="X1:Y1"/>
-    <mergeCell ref="AE2:AE3"/>
-    <mergeCell ref="AF2:AF3"/>
-    <mergeCell ref="AG2:AG3"/>
-    <mergeCell ref="AH2:AH3"/>
-    <mergeCell ref="AI2:AI3"/>
-    <mergeCell ref="AJ2:AJ3"/>
-    <mergeCell ref="Y2:Y3"/>
-    <mergeCell ref="Z2:Z3"/>
-    <mergeCell ref="AB2:AB3"/>
-    <mergeCell ref="AC2:AC3"/>
-    <mergeCell ref="AD2:AD3"/>
+    <mergeCell ref="CR1:CY1"/>
+    <mergeCell ref="F2:F3"/>
+    <mergeCell ref="G2:G3"/>
+    <mergeCell ref="R2:R3"/>
+    <mergeCell ref="AR2:AR3"/>
+    <mergeCell ref="AZ2:AZ3"/>
+    <mergeCell ref="BA2:BA3"/>
+    <mergeCell ref="BC2:BC3"/>
+    <mergeCell ref="BU2:BU3"/>
+    <mergeCell ref="CF2:CF3"/>
+    <mergeCell ref="CL2:CL3"/>
+    <mergeCell ref="CO2:CO3"/>
+    <mergeCell ref="CP2:CP3"/>
+    <mergeCell ref="CQ2:CQ3"/>
+    <mergeCell ref="CR2:CR3"/>
+    <mergeCell ref="CT2:CT3"/>
+    <mergeCell ref="CU2:CU3"/>
+    <mergeCell ref="CV2:CV3"/>
+    <mergeCell ref="CW2:CW3"/>
+    <mergeCell ref="CY2:CY3"/>
+    <mergeCell ref="AB1:AF1"/>
+    <mergeCell ref="AG1:AQ1"/>
+    <mergeCell ref="AR1:AS1"/>
+    <mergeCell ref="AT1:AX1"/>
     <mergeCell ref="AY1:BL1"/>
     <mergeCell ref="BN1:BX1"/>
     <mergeCell ref="BY1:CG1"/>
@@ -17796,30 +17888,64 @@
     <mergeCell ref="X2:X3"/>
     <mergeCell ref="L2:L3"/>
     <mergeCell ref="N2:N3"/>
-    <mergeCell ref="CR1:CY1"/>
-    <mergeCell ref="F2:F3"/>
-    <mergeCell ref="G2:G3"/>
-    <mergeCell ref="R2:R3"/>
-    <mergeCell ref="AR2:AR3"/>
-    <mergeCell ref="AZ2:AZ3"/>
-    <mergeCell ref="BA2:BA3"/>
-    <mergeCell ref="BC2:BC3"/>
-    <mergeCell ref="BU2:BU3"/>
-    <mergeCell ref="CF2:CF3"/>
-    <mergeCell ref="CL2:CL3"/>
-    <mergeCell ref="CO2:CO3"/>
-    <mergeCell ref="CP2:CP3"/>
-    <mergeCell ref="CQ2:CQ3"/>
-    <mergeCell ref="CR2:CR3"/>
-    <mergeCell ref="CT2:CT3"/>
-    <mergeCell ref="CU2:CU3"/>
-    <mergeCell ref="CV2:CV3"/>
-    <mergeCell ref="CW2:CW3"/>
-    <mergeCell ref="CY2:CY3"/>
-    <mergeCell ref="AB1:AF1"/>
-    <mergeCell ref="AG1:AQ1"/>
-    <mergeCell ref="AR1:AS1"/>
-    <mergeCell ref="AT1:AX1"/>
+    <mergeCell ref="Q2:Q3"/>
+    <mergeCell ref="T1:W1"/>
+    <mergeCell ref="X1:Y1"/>
+    <mergeCell ref="AE2:AE3"/>
+    <mergeCell ref="AF2:AF3"/>
+    <mergeCell ref="AG2:AG3"/>
+    <mergeCell ref="AH2:AH3"/>
+    <mergeCell ref="AI2:AI3"/>
+    <mergeCell ref="AJ2:AJ3"/>
+    <mergeCell ref="Y2:Y3"/>
+    <mergeCell ref="Z2:Z3"/>
+    <mergeCell ref="AB2:AB3"/>
+    <mergeCell ref="AC2:AC3"/>
+    <mergeCell ref="AD2:AD3"/>
+    <mergeCell ref="AQ2:AQ3"/>
+    <mergeCell ref="AS2:AS3"/>
+    <mergeCell ref="AT2:AT3"/>
+    <mergeCell ref="AU2:AU3"/>
+    <mergeCell ref="AV2:AV3"/>
+    <mergeCell ref="AW2:AW3"/>
+    <mergeCell ref="AK2:AK3"/>
+    <mergeCell ref="AL2:AL3"/>
+    <mergeCell ref="AM2:AM3"/>
+    <mergeCell ref="AN2:AN3"/>
+    <mergeCell ref="AO2:AO3"/>
+    <mergeCell ref="AP2:AP3"/>
+    <mergeCell ref="BG2:BG3"/>
+    <mergeCell ref="BH2:BH3"/>
+    <mergeCell ref="BI2:BI3"/>
+    <mergeCell ref="BJ2:BJ3"/>
+    <mergeCell ref="BK2:BK3"/>
+    <mergeCell ref="BL2:BL3"/>
+    <mergeCell ref="AX2:AX3"/>
+    <mergeCell ref="AY2:AY3"/>
+    <mergeCell ref="BB2:BB3"/>
+    <mergeCell ref="BD2:BD3"/>
+    <mergeCell ref="BF2:BF3"/>
+    <mergeCell ref="BV2:BV3"/>
+    <mergeCell ref="BW2:BW3"/>
+    <mergeCell ref="BX2:BX3"/>
+    <mergeCell ref="BY2:BY3"/>
+    <mergeCell ref="BO2:BO3"/>
+    <mergeCell ref="BQ2:BQ3"/>
+    <mergeCell ref="BR2:BR3"/>
+    <mergeCell ref="CN2:CN3"/>
+    <mergeCell ref="CG2:CG3"/>
+    <mergeCell ref="CI2:CI3"/>
+    <mergeCell ref="CJ2:CJ3"/>
+    <mergeCell ref="CK2:CK3"/>
+    <mergeCell ref="CM2:CM3"/>
+    <mergeCell ref="BZ2:BZ3"/>
+    <mergeCell ref="CA2:CA3"/>
+    <mergeCell ref="CB2:CB3"/>
+    <mergeCell ref="CC2:CC3"/>
+    <mergeCell ref="CD2:CD3"/>
+    <mergeCell ref="CE2:CE3"/>
+    <mergeCell ref="BS2:BS3"/>
+    <mergeCell ref="BT2:BT3"/>
   </mergeCells>
   <phoneticPr fontId="26" type="noConversion"/>
   <hyperlinks>
@@ -18057,7 +18183,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4F29D14F-5256-41EB-8E69-D00BD3A17764}">
   <dimension ref="A1:E13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
@@ -18301,10 +18427,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1F0720B9-F1C1-4E88-8345-0A7B8577FCEF}">
-  <dimension ref="A1:CS86"/>
+  <dimension ref="A1:CS91"/>
   <sheetViews>
-    <sheetView topLeftCell="CO43" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="CS86" sqref="CS86"/>
+    <sheetView tabSelected="1" topLeftCell="BT79" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="BZ94" sqref="BZ94"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -18456,492 +18582,492 @@
       <c r="A2" s="9" t="s">
         <v>115</v>
       </c>
-      <c r="B2" s="25" t="s">
+      <c r="B2" s="24" t="s">
         <v>90</v>
       </c>
-      <c r="C2" s="25" t="s">
+      <c r="C2" s="24" t="s">
         <v>109</v>
       </c>
-      <c r="D2" s="25" t="s">
+      <c r="D2" s="24" t="s">
         <v>89</v>
       </c>
-      <c r="E2" s="25" t="s">
+      <c r="E2" s="24" t="s">
         <v>345</v>
       </c>
-      <c r="F2" s="25" t="s">
+      <c r="F2" s="24" t="s">
         <v>106</v>
       </c>
-      <c r="G2" s="25" t="s">
+      <c r="G2" s="24" t="s">
         <v>56</v>
       </c>
-      <c r="H2" s="25" t="s">
+      <c r="H2" s="24" t="s">
         <v>48</v>
       </c>
-      <c r="I2" s="25" t="s">
+      <c r="I2" s="24" t="s">
         <v>62</v>
       </c>
-      <c r="J2" s="25" t="s">
+      <c r="J2" s="24" t="s">
         <v>112</v>
       </c>
-      <c r="K2" s="25" t="s">
+      <c r="K2" s="24" t="s">
         <v>67</v>
       </c>
-      <c r="L2" s="25" t="s">
+      <c r="L2" s="24" t="s">
         <v>77</v>
       </c>
-      <c r="M2" s="25" t="s">
+      <c r="M2" s="24" t="s">
         <v>346</v>
       </c>
-      <c r="N2" s="25" t="s">
+      <c r="N2" s="24" t="s">
         <v>111</v>
       </c>
-      <c r="O2" s="25" t="s">
+      <c r="O2" s="24" t="s">
         <v>79</v>
       </c>
-      <c r="P2" s="25" t="s">
+      <c r="P2" s="24" t="s">
         <v>104</v>
       </c>
-      <c r="Q2" s="25" t="s">
+      <c r="Q2" s="24" t="s">
         <v>94</v>
       </c>
       <c r="R2" s="9" t="s">
         <v>115</v>
       </c>
-      <c r="S2" s="25" t="s">
+      <c r="S2" s="24" t="s">
         <v>10</v>
       </c>
-      <c r="T2" s="25" t="s">
+      <c r="T2" s="24" t="s">
         <v>368</v>
       </c>
-      <c r="U2" s="25" t="s">
+      <c r="U2" s="24" t="s">
         <v>65</v>
       </c>
-      <c r="V2" s="25" t="s">
+      <c r="V2" s="24" t="s">
         <v>103</v>
       </c>
-      <c r="W2" s="25" t="s">
+      <c r="W2" s="24" t="s">
         <v>42</v>
       </c>
-      <c r="X2" s="25" t="s">
+      <c r="X2" s="24" t="s">
         <v>39</v>
       </c>
-      <c r="Y2" s="25" t="s">
+      <c r="Y2" s="24" t="s">
         <v>93</v>
       </c>
-      <c r="Z2" s="25" t="s">
+      <c r="Z2" s="24" t="s">
         <v>50</v>
       </c>
-      <c r="AA2" s="25" t="s">
+      <c r="AA2" s="24" t="s">
         <v>102</v>
       </c>
-      <c r="AB2" s="25" t="s">
+      <c r="AB2" s="24" t="s">
         <v>41</v>
       </c>
-      <c r="AC2" s="25" t="s">
+      <c r="AC2" s="24" t="s">
         <v>16</v>
       </c>
-      <c r="AD2" s="25" t="s">
+      <c r="AD2" s="24" t="s">
         <v>24</v>
       </c>
-      <c r="AE2" s="25" t="s">
+      <c r="AE2" s="24" t="s">
         <v>49</v>
       </c>
-      <c r="AF2" s="25" t="s">
+      <c r="AF2" s="24" t="s">
         <v>22</v>
       </c>
-      <c r="AG2" s="25" t="s">
+      <c r="AG2" s="24" t="s">
         <v>108</v>
       </c>
-      <c r="AH2" s="25" t="s">
+      <c r="AH2" s="24" t="s">
         <v>97</v>
       </c>
-      <c r="AI2" s="25" t="s">
+      <c r="AI2" s="24" t="s">
         <v>43</v>
       </c>
       <c r="AJ2" s="9" t="s">
         <v>115</v>
       </c>
-      <c r="AK2" s="25" t="s">
+      <c r="AK2" s="24" t="s">
         <v>47</v>
       </c>
-      <c r="AL2" s="25" t="s">
+      <c r="AL2" s="24" t="s">
         <v>23</v>
       </c>
-      <c r="AM2" s="25" t="s">
+      <c r="AM2" s="24" t="s">
         <v>138</v>
       </c>
-      <c r="AN2" s="25" t="s">
+      <c r="AN2" s="24" t="s">
         <v>63</v>
       </c>
-      <c r="AO2" s="25" t="s">
+      <c r="AO2" s="24" t="s">
         <v>29</v>
       </c>
-      <c r="AP2" s="25" t="s">
+      <c r="AP2" s="24" t="s">
         <v>18</v>
       </c>
-      <c r="AQ2" s="25" t="s">
+      <c r="AQ2" s="24" t="s">
         <v>35</v>
       </c>
-      <c r="AR2" s="25" t="s">
+      <c r="AR2" s="24" t="s">
         <v>38</v>
       </c>
-      <c r="AS2" s="25" t="s">
+      <c r="AS2" s="24" t="s">
         <v>28</v>
       </c>
-      <c r="AT2" s="25" t="s">
+      <c r="AT2" s="24" t="s">
         <v>87</v>
       </c>
-      <c r="AU2" s="25" t="s">
+      <c r="AU2" s="24" t="s">
         <v>98</v>
       </c>
-      <c r="AV2" s="25" t="s">
+      <c r="AV2" s="24" t="s">
         <v>37</v>
       </c>
-      <c r="AW2" s="25" t="s">
+      <c r="AW2" s="24" t="s">
         <v>4</v>
       </c>
-      <c r="AX2" s="25" t="s">
+      <c r="AX2" s="24" t="s">
         <v>26</v>
       </c>
-      <c r="AY2" s="25" t="s">
+      <c r="AY2" s="24" t="s">
         <v>81</v>
       </c>
-      <c r="AZ2" s="25" t="s">
+      <c r="AZ2" s="24" t="s">
         <v>51</v>
       </c>
-      <c r="BA2" s="25" t="s">
+      <c r="BA2" s="24" t="s">
         <v>78</v>
       </c>
-      <c r="BB2" s="25" t="s">
+      <c r="BB2" s="24" t="s">
         <v>52</v>
       </c>
-      <c r="BC2" s="25" t="s">
+      <c r="BC2" s="24" t="s">
         <v>15</v>
       </c>
-      <c r="BD2" s="25" t="s">
+      <c r="BD2" s="24" t="s">
         <v>54</v>
       </c>
-      <c r="BE2" s="25" t="s">
+      <c r="BE2" s="24" t="s">
         <v>32</v>
       </c>
-      <c r="BF2" s="25" t="s">
+      <c r="BF2" s="24" t="s">
         <v>11</v>
       </c>
-      <c r="BG2" s="25" t="s">
+      <c r="BG2" s="24" t="s">
         <v>347</v>
       </c>
       <c r="BH2" s="9" t="s">
         <v>115</v>
       </c>
-      <c r="BI2" s="25" t="s">
+      <c r="BI2" s="24" t="s">
         <v>61</v>
       </c>
-      <c r="BJ2" s="25" t="s">
+      <c r="BJ2" s="24" t="s">
         <v>348</v>
       </c>
-      <c r="BK2" s="25" t="s">
+      <c r="BK2" s="24" t="s">
         <v>59</v>
       </c>
-      <c r="BL2" s="25" t="s">
+      <c r="BL2" s="24" t="s">
         <v>75</v>
       </c>
-      <c r="BM2" s="25" t="s">
+      <c r="BM2" s="24" t="s">
         <v>27</v>
       </c>
-      <c r="BN2" s="25" t="s">
+      <c r="BN2" s="24" t="s">
         <v>25</v>
       </c>
       <c r="BO2" s="22" t="s">
         <v>88</v>
       </c>
-      <c r="BP2" s="25" t="s">
+      <c r="BP2" s="24" t="s">
         <v>68</v>
       </c>
-      <c r="BQ2" s="25" t="s">
+      <c r="BQ2" s="24" t="s">
         <v>19</v>
       </c>
-      <c r="BR2" s="25" t="s">
+      <c r="BR2" s="24" t="s">
         <v>30</v>
       </c>
-      <c r="BS2" s="25" t="s">
+      <c r="BS2" s="24" t="s">
         <v>36</v>
       </c>
-      <c r="BT2" s="25" t="s">
+      <c r="BT2" s="24" t="s">
         <v>20</v>
       </c>
-      <c r="BU2" s="25" t="s">
+      <c r="BU2" s="24" t="s">
         <v>57</v>
       </c>
-      <c r="BV2" s="25" t="s">
+      <c r="BV2" s="24" t="s">
         <v>13</v>
       </c>
-      <c r="BW2" s="25" t="s">
+      <c r="BW2" s="24" t="s">
         <v>17</v>
       </c>
-      <c r="BX2" s="25" t="s">
+      <c r="BX2" s="24" t="s">
         <v>369</v>
       </c>
-      <c r="BY2" s="25" t="s">
+      <c r="BY2" s="24" t="s">
         <v>74</v>
       </c>
-      <c r="BZ2" s="25" t="s">
+      <c r="BZ2" s="24" t="s">
         <v>70</v>
       </c>
-      <c r="CA2" s="25" t="s">
+      <c r="CA2" s="24" t="s">
         <v>66</v>
       </c>
-      <c r="CB2" s="25" t="s">
+      <c r="CB2" s="24" t="s">
         <v>34</v>
       </c>
-      <c r="CC2" s="25" t="s">
-        <v>1</v>
-      </c>
-      <c r="CD2" s="25" t="s">
+      <c r="CC2" s="24" t="s">
+        <v>1</v>
+      </c>
+      <c r="CD2" s="24" t="s">
         <v>92</v>
       </c>
-      <c r="CE2" s="25" t="s">
+      <c r="CE2" s="24" t="s">
         <v>71</v>
       </c>
-      <c r="CF2" s="25" t="s">
+      <c r="CF2" s="24" t="s">
         <v>12</v>
       </c>
-      <c r="CG2" s="25" t="s">
+      <c r="CG2" s="24" t="s">
         <v>73</v>
       </c>
-      <c r="CH2" s="25" t="s">
+      <c r="CH2" s="24" t="s">
         <v>53</v>
       </c>
-      <c r="CI2" s="25" t="s">
+      <c r="CI2" s="24" t="s">
         <v>40</v>
       </c>
-      <c r="CJ2" s="25" t="s">
+      <c r="CJ2" s="24" t="s">
         <v>2</v>
       </c>
-      <c r="CK2" s="25" t="s">
+      <c r="CK2" s="24" t="s">
         <v>8</v>
       </c>
-      <c r="CL2" s="25" t="s">
+      <c r="CL2" s="24" t="s">
         <v>9</v>
       </c>
-      <c r="CM2" s="25" t="s">
+      <c r="CM2" s="24" t="s">
         <v>5</v>
       </c>
-      <c r="CN2" s="25" t="s">
+      <c r="CN2" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="CO2" s="25" t="s">
+      <c r="CO2" s="24" t="s">
         <v>21</v>
       </c>
-      <c r="CP2" s="25" t="s">
+      <c r="CP2" s="24" t="s">
         <v>7</v>
       </c>
-      <c r="CQ2" s="25" t="s">
+      <c r="CQ2" s="24" t="s">
         <v>6</v>
       </c>
-      <c r="CR2" s="25" t="s">
+      <c r="CR2" s="24" t="s">
         <v>14</v>
       </c>
-      <c r="CS2" s="25" t="s">
+      <c r="CS2" s="24" t="s">
         <v>147</v>
       </c>
     </row>
     <row r="3" spans="1:97" x14ac:dyDescent="0.3">
       <c r="A3" s="20"/>
-      <c r="B3" s="25"/>
-      <c r="C3" s="25"/>
-      <c r="D3" s="25"/>
-      <c r="E3" s="25"/>
-      <c r="F3" s="25"/>
-      <c r="G3" s="25"/>
-      <c r="H3" s="25"/>
-      <c r="I3" s="25"/>
-      <c r="J3" s="25"/>
-      <c r="K3" s="25"/>
-      <c r="L3" s="25"/>
-      <c r="M3" s="25"/>
-      <c r="N3" s="25"/>
-      <c r="O3" s="25"/>
-      <c r="P3" s="25"/>
-      <c r="Q3" s="25"/>
+      <c r="B3" s="24"/>
+      <c r="C3" s="24"/>
+      <c r="D3" s="24"/>
+      <c r="E3" s="24"/>
+      <c r="F3" s="24"/>
+      <c r="G3" s="24"/>
+      <c r="H3" s="24"/>
+      <c r="I3" s="24"/>
+      <c r="J3" s="24"/>
+      <c r="K3" s="24"/>
+      <c r="L3" s="24"/>
+      <c r="M3" s="24"/>
+      <c r="N3" s="24"/>
+      <c r="O3" s="24"/>
+      <c r="P3" s="24"/>
+      <c r="Q3" s="24"/>
       <c r="R3" s="20"/>
-      <c r="S3" s="25"/>
-      <c r="T3" s="25"/>
-      <c r="U3" s="25"/>
-      <c r="V3" s="25"/>
-      <c r="W3" s="25"/>
-      <c r="X3" s="25"/>
-      <c r="Y3" s="25"/>
-      <c r="Z3" s="25"/>
-      <c r="AA3" s="25"/>
-      <c r="AB3" s="25"/>
-      <c r="AC3" s="25"/>
-      <c r="AD3" s="25"/>
-      <c r="AE3" s="25"/>
-      <c r="AF3" s="25"/>
-      <c r="AG3" s="25"/>
-      <c r="AH3" s="25"/>
-      <c r="AI3" s="25"/>
+      <c r="S3" s="24"/>
+      <c r="T3" s="24"/>
+      <c r="U3" s="24"/>
+      <c r="V3" s="24"/>
+      <c r="W3" s="24"/>
+      <c r="X3" s="24"/>
+      <c r="Y3" s="24"/>
+      <c r="Z3" s="24"/>
+      <c r="AA3" s="24"/>
+      <c r="AB3" s="24"/>
+      <c r="AC3" s="24"/>
+      <c r="AD3" s="24"/>
+      <c r="AE3" s="24"/>
+      <c r="AF3" s="24"/>
+      <c r="AG3" s="24"/>
+      <c r="AH3" s="24"/>
+      <c r="AI3" s="24"/>
       <c r="AJ3" s="20"/>
-      <c r="AK3" s="25"/>
-      <c r="AL3" s="25"/>
-      <c r="AM3" s="25"/>
-      <c r="AN3" s="25"/>
-      <c r="AO3" s="25"/>
-      <c r="AP3" s="25"/>
-      <c r="AQ3" s="25"/>
-      <c r="AR3" s="25"/>
-      <c r="AS3" s="25"/>
-      <c r="AT3" s="25"/>
-      <c r="AU3" s="25"/>
-      <c r="AV3" s="25"/>
-      <c r="AW3" s="25"/>
-      <c r="AX3" s="25"/>
-      <c r="AY3" s="25"/>
-      <c r="AZ3" s="25"/>
-      <c r="BA3" s="25"/>
-      <c r="BB3" s="25"/>
-      <c r="BC3" s="25"/>
-      <c r="BD3" s="25"/>
-      <c r="BE3" s="25"/>
-      <c r="BF3" s="25"/>
-      <c r="BG3" s="25"/>
+      <c r="AK3" s="24"/>
+      <c r="AL3" s="24"/>
+      <c r="AM3" s="24"/>
+      <c r="AN3" s="24"/>
+      <c r="AO3" s="24"/>
+      <c r="AP3" s="24"/>
+      <c r="AQ3" s="24"/>
+      <c r="AR3" s="24"/>
+      <c r="AS3" s="24"/>
+      <c r="AT3" s="24"/>
+      <c r="AU3" s="24"/>
+      <c r="AV3" s="24"/>
+      <c r="AW3" s="24"/>
+      <c r="AX3" s="24"/>
+      <c r="AY3" s="24"/>
+      <c r="AZ3" s="24"/>
+      <c r="BA3" s="24"/>
+      <c r="BB3" s="24"/>
+      <c r="BC3" s="24"/>
+      <c r="BD3" s="24"/>
+      <c r="BE3" s="24"/>
+      <c r="BF3" s="24"/>
+      <c r="BG3" s="24"/>
       <c r="BH3" s="20"/>
-      <c r="BI3" s="25"/>
-      <c r="BJ3" s="25"/>
-      <c r="BK3" s="25"/>
-      <c r="BL3" s="25"/>
-      <c r="BM3" s="25"/>
-      <c r="BN3" s="25"/>
+      <c r="BI3" s="24"/>
+      <c r="BJ3" s="24"/>
+      <c r="BK3" s="24"/>
+      <c r="BL3" s="24"/>
+      <c r="BM3" s="24"/>
+      <c r="BN3" s="24"/>
       <c r="BO3" s="22"/>
-      <c r="BP3" s="25"/>
-      <c r="BQ3" s="25"/>
-      <c r="BR3" s="25"/>
-      <c r="BS3" s="25"/>
-      <c r="BT3" s="25"/>
-      <c r="BU3" s="25"/>
-      <c r="BV3" s="25"/>
-      <c r="BW3" s="25"/>
-      <c r="BX3" s="25"/>
-      <c r="BY3" s="25"/>
-      <c r="BZ3" s="25"/>
-      <c r="CA3" s="25"/>
-      <c r="CB3" s="25"/>
-      <c r="CC3" s="25"/>
-      <c r="CD3" s="25"/>
-      <c r="CE3" s="25"/>
-      <c r="CF3" s="25"/>
-      <c r="CG3" s="25"/>
-      <c r="CH3" s="25"/>
-      <c r="CI3" s="25"/>
-      <c r="CJ3" s="25"/>
-      <c r="CK3" s="25"/>
-      <c r="CL3" s="25"/>
-      <c r="CM3" s="25"/>
-      <c r="CN3" s="25"/>
-      <c r="CO3" s="25"/>
-      <c r="CP3" s="25"/>
-      <c r="CQ3" s="25"/>
-      <c r="CR3" s="25"/>
-      <c r="CS3" s="25"/>
+      <c r="BP3" s="24"/>
+      <c r="BQ3" s="24"/>
+      <c r="BR3" s="24"/>
+      <c r="BS3" s="24"/>
+      <c r="BT3" s="24"/>
+      <c r="BU3" s="24"/>
+      <c r="BV3" s="24"/>
+      <c r="BW3" s="24"/>
+      <c r="BX3" s="24"/>
+      <c r="BY3" s="24"/>
+      <c r="BZ3" s="24"/>
+      <c r="CA3" s="24"/>
+      <c r="CB3" s="24"/>
+      <c r="CC3" s="24"/>
+      <c r="CD3" s="24"/>
+      <c r="CE3" s="24"/>
+      <c r="CF3" s="24"/>
+      <c r="CG3" s="24"/>
+      <c r="CH3" s="24"/>
+      <c r="CI3" s="24"/>
+      <c r="CJ3" s="24"/>
+      <c r="CK3" s="24"/>
+      <c r="CL3" s="24"/>
+      <c r="CM3" s="24"/>
+      <c r="CN3" s="24"/>
+      <c r="CO3" s="24"/>
+      <c r="CP3" s="24"/>
+      <c r="CQ3" s="24"/>
+      <c r="CR3" s="24"/>
+      <c r="CS3" s="24"/>
     </row>
     <row r="4" spans="1:97" x14ac:dyDescent="0.3">
       <c r="A4" s="9"/>
-      <c r="B4" s="25"/>
-      <c r="C4" s="25"/>
-      <c r="D4" s="25"/>
-      <c r="E4" s="25"/>
-      <c r="F4" s="25"/>
-      <c r="G4" s="25"/>
-      <c r="H4" s="25"/>
-      <c r="I4" s="25"/>
-      <c r="J4" s="25"/>
-      <c r="K4" s="25"/>
-      <c r="L4" s="25"/>
-      <c r="M4" s="25"/>
-      <c r="N4" s="25"/>
-      <c r="O4" s="25"/>
-      <c r="P4" s="25"/>
-      <c r="Q4" s="25"/>
+      <c r="B4" s="24"/>
+      <c r="C4" s="24"/>
+      <c r="D4" s="24"/>
+      <c r="E4" s="24"/>
+      <c r="F4" s="24"/>
+      <c r="G4" s="24"/>
+      <c r="H4" s="24"/>
+      <c r="I4" s="24"/>
+      <c r="J4" s="24"/>
+      <c r="K4" s="24"/>
+      <c r="L4" s="24"/>
+      <c r="M4" s="24"/>
+      <c r="N4" s="24"/>
+      <c r="O4" s="24"/>
+      <c r="P4" s="24"/>
+      <c r="Q4" s="24"/>
       <c r="R4" s="9"/>
-      <c r="S4" s="25"/>
-      <c r="T4" s="25"/>
-      <c r="U4" s="25"/>
-      <c r="V4" s="25"/>
-      <c r="W4" s="25"/>
-      <c r="X4" s="25"/>
-      <c r="Y4" s="25"/>
-      <c r="Z4" s="25"/>
-      <c r="AA4" s="25"/>
-      <c r="AB4" s="25"/>
-      <c r="AC4" s="25"/>
-      <c r="AD4" s="25"/>
-      <c r="AE4" s="25"/>
-      <c r="AF4" s="25"/>
-      <c r="AG4" s="25"/>
-      <c r="AH4" s="25"/>
-      <c r="AI4" s="25"/>
+      <c r="S4" s="24"/>
+      <c r="T4" s="24"/>
+      <c r="U4" s="24"/>
+      <c r="V4" s="24"/>
+      <c r="W4" s="24"/>
+      <c r="X4" s="24"/>
+      <c r="Y4" s="24"/>
+      <c r="Z4" s="24"/>
+      <c r="AA4" s="24"/>
+      <c r="AB4" s="24"/>
+      <c r="AC4" s="24"/>
+      <c r="AD4" s="24"/>
+      <c r="AE4" s="24"/>
+      <c r="AF4" s="24"/>
+      <c r="AG4" s="24"/>
+      <c r="AH4" s="24"/>
+      <c r="AI4" s="24"/>
       <c r="AJ4" s="9"/>
-      <c r="AK4" s="25"/>
-      <c r="AL4" s="25"/>
-      <c r="AM4" s="25"/>
-      <c r="AN4" s="25"/>
-      <c r="AO4" s="25"/>
-      <c r="AP4" s="25"/>
-      <c r="AQ4" s="25"/>
-      <c r="AR4" s="25"/>
-      <c r="AS4" s="25"/>
-      <c r="AT4" s="25"/>
-      <c r="AU4" s="25"/>
-      <c r="AV4" s="25"/>
-      <c r="AW4" s="25"/>
-      <c r="AX4" s="25"/>
-      <c r="AY4" s="25"/>
-      <c r="AZ4" s="25"/>
-      <c r="BA4" s="25"/>
-      <c r="BB4" s="25"/>
-      <c r="BC4" s="25"/>
-      <c r="BD4" s="25"/>
-      <c r="BE4" s="25"/>
-      <c r="BF4" s="25"/>
-      <c r="BG4" s="25"/>
+      <c r="AK4" s="24"/>
+      <c r="AL4" s="24"/>
+      <c r="AM4" s="24"/>
+      <c r="AN4" s="24"/>
+      <c r="AO4" s="24"/>
+      <c r="AP4" s="24"/>
+      <c r="AQ4" s="24"/>
+      <c r="AR4" s="24"/>
+      <c r="AS4" s="24"/>
+      <c r="AT4" s="24"/>
+      <c r="AU4" s="24"/>
+      <c r="AV4" s="24"/>
+      <c r="AW4" s="24"/>
+      <c r="AX4" s="24"/>
+      <c r="AY4" s="24"/>
+      <c r="AZ4" s="24"/>
+      <c r="BA4" s="24"/>
+      <c r="BB4" s="24"/>
+      <c r="BC4" s="24"/>
+      <c r="BD4" s="24"/>
+      <c r="BE4" s="24"/>
+      <c r="BF4" s="24"/>
+      <c r="BG4" s="24"/>
       <c r="BH4" s="9"/>
-      <c r="BI4" s="25"/>
-      <c r="BJ4" s="25"/>
-      <c r="BK4" s="25"/>
-      <c r="BL4" s="25"/>
-      <c r="BM4" s="25"/>
-      <c r="BN4" s="25"/>
+      <c r="BI4" s="24"/>
+      <c r="BJ4" s="24"/>
+      <c r="BK4" s="24"/>
+      <c r="BL4" s="24"/>
+      <c r="BM4" s="24"/>
+      <c r="BN4" s="24"/>
       <c r="BO4" s="22"/>
-      <c r="BP4" s="25"/>
-      <c r="BQ4" s="25"/>
-      <c r="BR4" s="25"/>
-      <c r="BS4" s="25"/>
-      <c r="BT4" s="25"/>
-      <c r="BU4" s="25"/>
-      <c r="BV4" s="25"/>
-      <c r="BW4" s="25"/>
-      <c r="BX4" s="25"/>
-      <c r="BY4" s="25"/>
-      <c r="BZ4" s="25"/>
-      <c r="CA4" s="25"/>
-      <c r="CB4" s="25"/>
-      <c r="CC4" s="25"/>
-      <c r="CD4" s="25"/>
-      <c r="CE4" s="25"/>
-      <c r="CF4" s="25"/>
-      <c r="CG4" s="25"/>
-      <c r="CH4" s="25"/>
-      <c r="CI4" s="25"/>
-      <c r="CJ4" s="25"/>
-      <c r="CK4" s="25"/>
-      <c r="CL4" s="25"/>
-      <c r="CM4" s="25"/>
-      <c r="CN4" s="25"/>
-      <c r="CO4" s="25"/>
-      <c r="CP4" s="25"/>
-      <c r="CQ4" s="25"/>
-      <c r="CR4" s="25"/>
-      <c r="CS4" s="25"/>
+      <c r="BP4" s="24"/>
+      <c r="BQ4" s="24"/>
+      <c r="BR4" s="24"/>
+      <c r="BS4" s="24"/>
+      <c r="BT4" s="24"/>
+      <c r="BU4" s="24"/>
+      <c r="BV4" s="24"/>
+      <c r="BW4" s="24"/>
+      <c r="BX4" s="24"/>
+      <c r="BY4" s="24"/>
+      <c r="BZ4" s="24"/>
+      <c r="CA4" s="24"/>
+      <c r="CB4" s="24"/>
+      <c r="CC4" s="24"/>
+      <c r="CD4" s="24"/>
+      <c r="CE4" s="24"/>
+      <c r="CF4" s="24"/>
+      <c r="CG4" s="24"/>
+      <c r="CH4" s="24"/>
+      <c r="CI4" s="24"/>
+      <c r="CJ4" s="24"/>
+      <c r="CK4" s="24"/>
+      <c r="CL4" s="24"/>
+      <c r="CM4" s="24"/>
+      <c r="CN4" s="24"/>
+      <c r="CO4" s="24"/>
+      <c r="CP4" s="24"/>
+      <c r="CQ4" s="24"/>
+      <c r="CR4" s="24"/>
+      <c r="CS4" s="24"/>
     </row>
     <row r="5" spans="1:97" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A5" s="20" t="s">
@@ -27576,6 +27702,9 @@
       <c r="CM84" s="10">
         <v>1341</v>
       </c>
+      <c r="CN84" s="16">
+        <v>258</v>
+      </c>
     </row>
     <row r="85" spans="1:97" x14ac:dyDescent="0.3">
       <c r="A85" s="10" t="s">
@@ -27596,6 +27725,9 @@
       <c r="CM85" s="10">
         <v>987</v>
       </c>
+      <c r="CN85" s="16">
+        <v>129</v>
+      </c>
     </row>
     <row r="86" spans="1:97" x14ac:dyDescent="0.3">
       <c r="A86" s="10" t="s">
@@ -27616,9 +27748,211 @@
       <c r="CM86" s="10">
         <v>635</v>
       </c>
+      <c r="CN86" s="16">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="87" spans="1:97" x14ac:dyDescent="0.3">
+      <c r="A87" s="10" t="s">
+        <v>379</v>
+      </c>
+      <c r="T87" s="10">
+        <v>1528</v>
+      </c>
+      <c r="BX87" s="10">
+        <v>737</v>
+      </c>
+      <c r="CC87" s="10">
+        <v>431</v>
+      </c>
+      <c r="CJ87" s="10">
+        <v>603</v>
+      </c>
+      <c r="CM87" s="10">
+        <v>561</v>
+      </c>
+      <c r="CN87" s="16">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="88" spans="1:97" x14ac:dyDescent="0.3">
+      <c r="A88" s="10" t="s">
+        <v>380</v>
+      </c>
+      <c r="T88" s="10">
+        <v>1535</v>
+      </c>
+      <c r="BX88" s="10">
+        <v>717</v>
+      </c>
+      <c r="CC88" s="10">
+        <v>566</v>
+      </c>
+      <c r="CJ88" s="10">
+        <v>547</v>
+      </c>
+      <c r="CM88" s="10">
+        <v>574</v>
+      </c>
+      <c r="CN88" s="16">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="89" spans="1:97" x14ac:dyDescent="0.3">
+      <c r="A89" s="10" t="s">
+        <v>381</v>
+      </c>
+      <c r="T89" s="10">
+        <v>6185</v>
+      </c>
+      <c r="BX89" s="10">
+        <v>778</v>
+      </c>
+      <c r="CC89" s="10">
+        <v>602</v>
+      </c>
+      <c r="CJ89" s="10">
+        <v>499</v>
+      </c>
+      <c r="CM89" s="10">
+        <v>762</v>
+      </c>
+      <c r="CN89" s="16">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="90" spans="1:97" x14ac:dyDescent="0.3">
+      <c r="A90" s="10" t="s">
+        <v>382</v>
+      </c>
+      <c r="T90" s="10">
+        <v>2618</v>
+      </c>
+      <c r="BX90" s="10">
+        <v>761</v>
+      </c>
+      <c r="CC90" s="10">
+        <v>578</v>
+      </c>
+      <c r="CJ90" s="10">
+        <v>557</v>
+      </c>
+      <c r="CM90" s="10">
+        <v>1438</v>
+      </c>
+      <c r="CN90" s="16">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="91" spans="1:97" x14ac:dyDescent="0.3">
+      <c r="A91" s="10" t="s">
+        <v>383</v>
+      </c>
+      <c r="T91" s="10">
+        <v>2174</v>
+      </c>
+      <c r="BX91" s="10">
+        <v>861</v>
+      </c>
+      <c r="CC91" s="10">
+        <v>525</v>
+      </c>
+      <c r="CJ91" s="10">
+        <v>503</v>
+      </c>
+      <c r="CM91" s="10">
+        <v>753</v>
+      </c>
+      <c r="CN91" s="16">
+        <v>248</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="108">
+    <mergeCell ref="CR2:CR4"/>
+    <mergeCell ref="CS2:CS4"/>
+    <mergeCell ref="CL2:CL4"/>
+    <mergeCell ref="CM2:CM4"/>
+    <mergeCell ref="CN2:CN4"/>
+    <mergeCell ref="CO2:CO4"/>
+    <mergeCell ref="CP2:CP4"/>
+    <mergeCell ref="CQ2:CQ4"/>
+    <mergeCell ref="CF2:CF4"/>
+    <mergeCell ref="CG2:CG4"/>
+    <mergeCell ref="CH2:CH4"/>
+    <mergeCell ref="CI2:CI4"/>
+    <mergeCell ref="CJ2:CJ4"/>
+    <mergeCell ref="CK2:CK4"/>
+    <mergeCell ref="CB2:CB4"/>
+    <mergeCell ref="CC2:CC4"/>
+    <mergeCell ref="CD2:CD4"/>
+    <mergeCell ref="CE2:CE4"/>
+    <mergeCell ref="BT2:BT4"/>
+    <mergeCell ref="BU2:BU4"/>
+    <mergeCell ref="BV2:BV4"/>
+    <mergeCell ref="BW2:BW4"/>
+    <mergeCell ref="BX2:BX4"/>
+    <mergeCell ref="BY2:BY4"/>
+    <mergeCell ref="BZ2:BZ4"/>
+    <mergeCell ref="CA2:CA4"/>
+    <mergeCell ref="BM2:BM4"/>
+    <mergeCell ref="BN2:BN4"/>
+    <mergeCell ref="BP2:BP4"/>
+    <mergeCell ref="BQ2:BQ4"/>
+    <mergeCell ref="BR2:BR4"/>
+    <mergeCell ref="BS2:BS4"/>
+    <mergeCell ref="BF2:BF4"/>
+    <mergeCell ref="BG2:BG4"/>
+    <mergeCell ref="BI2:BI4"/>
+    <mergeCell ref="BJ2:BJ4"/>
+    <mergeCell ref="BK2:BK4"/>
+    <mergeCell ref="BL2:BL4"/>
+    <mergeCell ref="AZ2:AZ4"/>
+    <mergeCell ref="BA2:BA4"/>
+    <mergeCell ref="BB2:BB4"/>
+    <mergeCell ref="BC2:BC4"/>
+    <mergeCell ref="BD2:BD4"/>
+    <mergeCell ref="BE2:BE4"/>
+    <mergeCell ref="AT2:AT4"/>
+    <mergeCell ref="AU2:AU4"/>
+    <mergeCell ref="AV2:AV4"/>
+    <mergeCell ref="AW2:AW4"/>
+    <mergeCell ref="AX2:AX4"/>
+    <mergeCell ref="AY2:AY4"/>
+    <mergeCell ref="AN2:AN4"/>
+    <mergeCell ref="AO2:AO4"/>
+    <mergeCell ref="AP2:AP4"/>
+    <mergeCell ref="AQ2:AQ4"/>
+    <mergeCell ref="AR2:AR4"/>
+    <mergeCell ref="AS2:AS4"/>
+    <mergeCell ref="AG2:AG4"/>
+    <mergeCell ref="AH2:AH4"/>
+    <mergeCell ref="AI2:AI4"/>
+    <mergeCell ref="AK2:AK4"/>
+    <mergeCell ref="AL2:AL4"/>
+    <mergeCell ref="AM2:AM4"/>
+    <mergeCell ref="AA2:AA4"/>
+    <mergeCell ref="AB2:AB4"/>
+    <mergeCell ref="AC2:AC4"/>
+    <mergeCell ref="AD2:AD4"/>
+    <mergeCell ref="AE2:AE4"/>
+    <mergeCell ref="AF2:AF4"/>
+    <mergeCell ref="U2:U4"/>
+    <mergeCell ref="V2:V4"/>
+    <mergeCell ref="W2:W4"/>
+    <mergeCell ref="X2:X4"/>
+    <mergeCell ref="Y2:Y4"/>
+    <mergeCell ref="Z2:Z4"/>
+    <mergeCell ref="P2:P4"/>
+    <mergeCell ref="Q2:Q4"/>
+    <mergeCell ref="S2:S4"/>
+    <mergeCell ref="T2:T4"/>
+    <mergeCell ref="H2:H4"/>
+    <mergeCell ref="I2:I4"/>
+    <mergeCell ref="J2:J4"/>
+    <mergeCell ref="K2:K4"/>
+    <mergeCell ref="L2:L4"/>
+    <mergeCell ref="M2:M4"/>
     <mergeCell ref="BI1:BP1"/>
     <mergeCell ref="BQ1:BX1"/>
     <mergeCell ref="BY1:CJ1"/>
@@ -27643,90 +27977,6 @@
     <mergeCell ref="U1:X1"/>
     <mergeCell ref="N2:N4"/>
     <mergeCell ref="O2:O4"/>
-    <mergeCell ref="P2:P4"/>
-    <mergeCell ref="Q2:Q4"/>
-    <mergeCell ref="S2:S4"/>
-    <mergeCell ref="T2:T4"/>
-    <mergeCell ref="H2:H4"/>
-    <mergeCell ref="I2:I4"/>
-    <mergeCell ref="J2:J4"/>
-    <mergeCell ref="K2:K4"/>
-    <mergeCell ref="L2:L4"/>
-    <mergeCell ref="M2:M4"/>
-    <mergeCell ref="AA2:AA4"/>
-    <mergeCell ref="AB2:AB4"/>
-    <mergeCell ref="AC2:AC4"/>
-    <mergeCell ref="AD2:AD4"/>
-    <mergeCell ref="AE2:AE4"/>
-    <mergeCell ref="AF2:AF4"/>
-    <mergeCell ref="U2:U4"/>
-    <mergeCell ref="V2:V4"/>
-    <mergeCell ref="W2:W4"/>
-    <mergeCell ref="X2:X4"/>
-    <mergeCell ref="Y2:Y4"/>
-    <mergeCell ref="Z2:Z4"/>
-    <mergeCell ref="AN2:AN4"/>
-    <mergeCell ref="AO2:AO4"/>
-    <mergeCell ref="AP2:AP4"/>
-    <mergeCell ref="AQ2:AQ4"/>
-    <mergeCell ref="AR2:AR4"/>
-    <mergeCell ref="AS2:AS4"/>
-    <mergeCell ref="AG2:AG4"/>
-    <mergeCell ref="AH2:AH4"/>
-    <mergeCell ref="AI2:AI4"/>
-    <mergeCell ref="AK2:AK4"/>
-    <mergeCell ref="AL2:AL4"/>
-    <mergeCell ref="AM2:AM4"/>
-    <mergeCell ref="AZ2:AZ4"/>
-    <mergeCell ref="BA2:BA4"/>
-    <mergeCell ref="BB2:BB4"/>
-    <mergeCell ref="BC2:BC4"/>
-    <mergeCell ref="BD2:BD4"/>
-    <mergeCell ref="BE2:BE4"/>
-    <mergeCell ref="AT2:AT4"/>
-    <mergeCell ref="AU2:AU4"/>
-    <mergeCell ref="AV2:AV4"/>
-    <mergeCell ref="AW2:AW4"/>
-    <mergeCell ref="AX2:AX4"/>
-    <mergeCell ref="AY2:AY4"/>
-    <mergeCell ref="BM2:BM4"/>
-    <mergeCell ref="BN2:BN4"/>
-    <mergeCell ref="BP2:BP4"/>
-    <mergeCell ref="BQ2:BQ4"/>
-    <mergeCell ref="BR2:BR4"/>
-    <mergeCell ref="BS2:BS4"/>
-    <mergeCell ref="BF2:BF4"/>
-    <mergeCell ref="BG2:BG4"/>
-    <mergeCell ref="BI2:BI4"/>
-    <mergeCell ref="BJ2:BJ4"/>
-    <mergeCell ref="BK2:BK4"/>
-    <mergeCell ref="BL2:BL4"/>
-    <mergeCell ref="CB2:CB4"/>
-    <mergeCell ref="CC2:CC4"/>
-    <mergeCell ref="CD2:CD4"/>
-    <mergeCell ref="CE2:CE4"/>
-    <mergeCell ref="BT2:BT4"/>
-    <mergeCell ref="BU2:BU4"/>
-    <mergeCell ref="BV2:BV4"/>
-    <mergeCell ref="BW2:BW4"/>
-    <mergeCell ref="BX2:BX4"/>
-    <mergeCell ref="BY2:BY4"/>
-    <mergeCell ref="BZ2:BZ4"/>
-    <mergeCell ref="CA2:CA4"/>
-    <mergeCell ref="CR2:CR4"/>
-    <mergeCell ref="CS2:CS4"/>
-    <mergeCell ref="CL2:CL4"/>
-    <mergeCell ref="CM2:CM4"/>
-    <mergeCell ref="CN2:CN4"/>
-    <mergeCell ref="CO2:CO4"/>
-    <mergeCell ref="CP2:CP4"/>
-    <mergeCell ref="CQ2:CQ4"/>
-    <mergeCell ref="CF2:CF4"/>
-    <mergeCell ref="CG2:CG4"/>
-    <mergeCell ref="CH2:CH4"/>
-    <mergeCell ref="CI2:CI4"/>
-    <mergeCell ref="CJ2:CJ4"/>
-    <mergeCell ref="CK2:CK4"/>
   </mergeCells>
   <phoneticPr fontId="26" type="noConversion"/>
   <hyperlinks>
@@ -27845,187 +28095,187 @@
       <c r="A1" s="17" t="s">
         <v>114</v>
       </c>
-      <c r="B1" s="24" t="s">
+      <c r="B1" s="25" t="s">
         <v>116</v>
       </c>
-      <c r="C1" s="24"/>
-      <c r="D1" s="24"/>
-      <c r="E1" s="24"/>
-      <c r="F1" s="24"/>
-      <c r="G1" s="24"/>
-      <c r="H1" s="24"/>
-      <c r="I1" s="24"/>
-      <c r="J1" s="24"/>
-      <c r="K1" s="24"/>
-      <c r="L1" s="24"/>
-      <c r="M1" s="24"/>
-      <c r="N1" s="24"/>
-      <c r="O1" s="24" t="s">
+      <c r="C1" s="25"/>
+      <c r="D1" s="25"/>
+      <c r="E1" s="25"/>
+      <c r="F1" s="25"/>
+      <c r="G1" s="25"/>
+      <c r="H1" s="25"/>
+      <c r="I1" s="25"/>
+      <c r="J1" s="25"/>
+      <c r="K1" s="25"/>
+      <c r="L1" s="25"/>
+      <c r="M1" s="25"/>
+      <c r="N1" s="25"/>
+      <c r="O1" s="25" t="s">
         <v>117</v>
       </c>
-      <c r="P1" s="24"/>
+      <c r="P1" s="25"/>
       <c r="Q1" s="17" t="s">
         <v>118</v>
       </c>
-      <c r="R1" s="24" t="s">
+      <c r="R1" s="25" t="s">
         <v>119</v>
       </c>
-      <c r="S1" s="24"/>
-      <c r="T1" s="24" t="s">
+      <c r="S1" s="25"/>
+      <c r="T1" s="25" t="s">
         <v>120</v>
       </c>
-      <c r="U1" s="24"/>
-      <c r="V1" s="24"/>
-      <c r="W1" s="24"/>
-      <c r="X1" s="24" t="s">
+      <c r="U1" s="25"/>
+      <c r="V1" s="25"/>
+      <c r="W1" s="25"/>
+      <c r="X1" s="25" t="s">
         <v>121</v>
       </c>
-      <c r="Y1" s="24"/>
+      <c r="Y1" s="25"/>
       <c r="Z1" s="17" t="s">
         <v>122</v>
       </c>
       <c r="AA1" s="17" t="s">
         <v>114</v>
       </c>
-      <c r="AB1" s="24" t="s">
+      <c r="AB1" s="25" t="s">
         <v>123</v>
       </c>
-      <c r="AC1" s="24"/>
-      <c r="AD1" s="24"/>
-      <c r="AE1" s="24"/>
-      <c r="AF1" s="24"/>
-      <c r="AG1" s="24" t="s">
+      <c r="AC1" s="25"/>
+      <c r="AD1" s="25"/>
+      <c r="AE1" s="25"/>
+      <c r="AF1" s="25"/>
+      <c r="AG1" s="25" t="s">
         <v>124</v>
       </c>
-      <c r="AH1" s="24"/>
-      <c r="AI1" s="24"/>
-      <c r="AJ1" s="24"/>
-      <c r="AK1" s="24"/>
-      <c r="AL1" s="24"/>
-      <c r="AM1" s="24"/>
-      <c r="AN1" s="24"/>
-      <c r="AO1" s="24"/>
-      <c r="AP1" s="24"/>
-      <c r="AQ1" s="24"/>
-      <c r="AR1" s="24" t="s">
+      <c r="AH1" s="25"/>
+      <c r="AI1" s="25"/>
+      <c r="AJ1" s="25"/>
+      <c r="AK1" s="25"/>
+      <c r="AL1" s="25"/>
+      <c r="AM1" s="25"/>
+      <c r="AN1" s="25"/>
+      <c r="AO1" s="25"/>
+      <c r="AP1" s="25"/>
+      <c r="AQ1" s="25"/>
+      <c r="AR1" s="25" t="s">
         <v>125</v>
       </c>
-      <c r="AS1" s="24"/>
-      <c r="AT1" s="24" t="s">
+      <c r="AS1" s="25"/>
+      <c r="AT1" s="25" t="s">
         <v>126</v>
       </c>
-      <c r="AU1" s="24"/>
-      <c r="AV1" s="24"/>
-      <c r="AW1" s="24"/>
-      <c r="AX1" s="24"/>
-      <c r="AY1" s="24" t="s">
+      <c r="AU1" s="25"/>
+      <c r="AV1" s="25"/>
+      <c r="AW1" s="25"/>
+      <c r="AX1" s="25"/>
+      <c r="AY1" s="25" t="s">
         <v>127</v>
       </c>
-      <c r="AZ1" s="24"/>
-      <c r="BA1" s="24"/>
-      <c r="BB1" s="24"/>
-      <c r="BC1" s="24"/>
-      <c r="BD1" s="24"/>
-      <c r="BE1" s="24"/>
-      <c r="BF1" s="24"/>
-      <c r="BG1" s="24"/>
-      <c r="BH1" s="24"/>
-      <c r="BI1" s="24"/>
-      <c r="BJ1" s="24"/>
-      <c r="BK1" s="24"/>
-      <c r="BL1" s="24"/>
+      <c r="AZ1" s="25"/>
+      <c r="BA1" s="25"/>
+      <c r="BB1" s="25"/>
+      <c r="BC1" s="25"/>
+      <c r="BD1" s="25"/>
+      <c r="BE1" s="25"/>
+      <c r="BF1" s="25"/>
+      <c r="BG1" s="25"/>
+      <c r="BH1" s="25"/>
+      <c r="BI1" s="25"/>
+      <c r="BJ1" s="25"/>
+      <c r="BK1" s="25"/>
+      <c r="BL1" s="25"/>
       <c r="BM1" s="17" t="s">
         <v>114</v>
       </c>
-      <c r="BN1" s="24" t="s">
+      <c r="BN1" s="25" t="s">
         <v>128</v>
       </c>
-      <c r="BO1" s="24"/>
-      <c r="BP1" s="24"/>
-      <c r="BQ1" s="24"/>
-      <c r="BR1" s="24"/>
-      <c r="BS1" s="24"/>
-      <c r="BT1" s="24"/>
-      <c r="BU1" s="24"/>
-      <c r="BV1" s="24"/>
-      <c r="BW1" s="24"/>
-      <c r="BX1" s="24"/>
-      <c r="BY1" s="24" t="s">
+      <c r="BO1" s="25"/>
+      <c r="BP1" s="25"/>
+      <c r="BQ1" s="25"/>
+      <c r="BR1" s="25"/>
+      <c r="BS1" s="25"/>
+      <c r="BT1" s="25"/>
+      <c r="BU1" s="25"/>
+      <c r="BV1" s="25"/>
+      <c r="BW1" s="25"/>
+      <c r="BX1" s="25"/>
+      <c r="BY1" s="25" t="s">
         <v>129</v>
       </c>
-      <c r="BZ1" s="24"/>
-      <c r="CA1" s="24"/>
-      <c r="CB1" s="24"/>
-      <c r="CC1" s="24"/>
-      <c r="CD1" s="24"/>
-      <c r="CE1" s="24"/>
-      <c r="CF1" s="24"/>
-      <c r="CG1" s="24"/>
-      <c r="CH1" s="24" t="s">
+      <c r="BZ1" s="25"/>
+      <c r="CA1" s="25"/>
+      <c r="CB1" s="25"/>
+      <c r="CC1" s="25"/>
+      <c r="CD1" s="25"/>
+      <c r="CE1" s="25"/>
+      <c r="CF1" s="25"/>
+      <c r="CG1" s="25"/>
+      <c r="CH1" s="25" t="s">
         <v>130</v>
       </c>
-      <c r="CI1" s="24"/>
-      <c r="CJ1" s="24"/>
-      <c r="CK1" s="24"/>
-      <c r="CL1" s="24"/>
-      <c r="CM1" s="24"/>
-      <c r="CN1" s="24"/>
-      <c r="CO1" s="24"/>
-      <c r="CP1" s="24"/>
-      <c r="CQ1" s="24"/>
-      <c r="CR1" s="24" t="s">
+      <c r="CI1" s="25"/>
+      <c r="CJ1" s="25"/>
+      <c r="CK1" s="25"/>
+      <c r="CL1" s="25"/>
+      <c r="CM1" s="25"/>
+      <c r="CN1" s="25"/>
+      <c r="CO1" s="25"/>
+      <c r="CP1" s="25"/>
+      <c r="CQ1" s="25"/>
+      <c r="CR1" s="25" t="s">
         <v>131</v>
       </c>
-      <c r="CS1" s="24"/>
-      <c r="CT1" s="24"/>
-      <c r="CU1" s="24"/>
-      <c r="CV1" s="24"/>
-      <c r="CW1" s="24"/>
-      <c r="CX1" s="24"/>
-      <c r="CY1" s="24"/>
+      <c r="CS1" s="25"/>
+      <c r="CT1" s="25"/>
+      <c r="CU1" s="25"/>
+      <c r="CV1" s="25"/>
+      <c r="CW1" s="25"/>
+      <c r="CX1" s="25"/>
+      <c r="CY1" s="25"/>
       <c r="CZ1" s="17"/>
     </row>
     <row r="2" spans="1:104" ht="102" x14ac:dyDescent="0.3">
       <c r="A2" s="17" t="s">
         <v>115</v>
       </c>
-      <c r="B2" s="25" t="s">
+      <c r="B2" s="24" t="s">
         <v>41</v>
       </c>
-      <c r="C2" s="25" t="s">
+      <c r="C2" s="24" t="s">
         <v>24</v>
       </c>
-      <c r="D2" s="25" t="s">
+      <c r="D2" s="24" t="s">
         <v>22</v>
       </c>
-      <c r="E2" s="25" t="s">
+      <c r="E2" s="24" t="s">
         <v>16</v>
       </c>
-      <c r="F2" s="25" t="s">
+      <c r="F2" s="24" t="s">
         <v>43</v>
       </c>
-      <c r="G2" s="25" t="s">
+      <c r="G2" s="24" t="s">
         <v>49</v>
       </c>
-      <c r="H2" s="25" t="s">
+      <c r="H2" s="24" t="s">
         <v>64</v>
       </c>
-      <c r="I2" s="25" t="s">
+      <c r="I2" s="24" t="s">
         <v>84</v>
       </c>
-      <c r="J2" s="25" t="s">
+      <c r="J2" s="24" t="s">
         <v>95</v>
       </c>
-      <c r="K2" s="25" t="s">
+      <c r="K2" s="24" t="s">
         <v>97</v>
       </c>
-      <c r="L2" s="25" t="s">
+      <c r="L2" s="24" t="s">
         <v>101</v>
       </c>
-      <c r="M2" s="25" t="s">
+      <c r="M2" s="24" t="s">
         <v>108</v>
       </c>
-      <c r="N2" s="25" t="s">
+      <c r="N2" s="24" t="s">
         <v>105</v>
       </c>
       <c r="O2" s="19" t="s">
@@ -28034,148 +28284,148 @@
       <c r="P2" s="19" t="s">
         <v>134</v>
       </c>
-      <c r="Q2" s="25" t="s">
+      <c r="Q2" s="24" t="s">
         <v>42</v>
       </c>
-      <c r="R2" s="25" t="s">
+      <c r="R2" s="24" t="s">
         <v>136</v>
       </c>
-      <c r="S2" s="25" t="s">
+      <c r="S2" s="24" t="s">
         <v>10</v>
       </c>
-      <c r="T2" s="25" t="s">
+      <c r="T2" s="24" t="s">
         <v>48</v>
       </c>
-      <c r="U2" s="25" t="s">
+      <c r="U2" s="24" t="s">
         <v>56</v>
       </c>
-      <c r="V2" s="25" t="s">
+      <c r="V2" s="24" t="s">
         <v>67</v>
       </c>
-      <c r="W2" s="25" t="s">
+      <c r="W2" s="24" t="s">
         <v>62</v>
       </c>
-      <c r="X2" s="25" t="s">
+      <c r="X2" s="24" t="s">
         <v>94</v>
       </c>
-      <c r="Y2" s="25" t="s">
+      <c r="Y2" s="24" t="s">
         <v>82</v>
       </c>
-      <c r="Z2" s="25" t="s">
+      <c r="Z2" s="24" t="s">
         <v>33</v>
       </c>
       <c r="AA2" s="17" t="s">
         <v>115</v>
       </c>
-      <c r="AB2" s="25" t="s">
+      <c r="AB2" s="24" t="s">
         <v>47</v>
       </c>
-      <c r="AC2" s="25" t="s">
+      <c r="AC2" s="24" t="s">
         <v>137</v>
       </c>
-      <c r="AD2" s="25" t="s">
+      <c r="AD2" s="24" t="s">
         <v>63</v>
       </c>
-      <c r="AE2" s="25" t="s">
+      <c r="AE2" s="24" t="s">
         <v>138</v>
       </c>
-      <c r="AF2" s="25" t="s">
+      <c r="AF2" s="24" t="s">
         <v>23</v>
       </c>
-      <c r="AG2" s="25" t="s">
+      <c r="AG2" s="24" t="s">
         <v>76</v>
       </c>
-      <c r="AH2" s="25" t="s">
+      <c r="AH2" s="24" t="s">
         <v>86</v>
       </c>
-      <c r="AI2" s="25" t="s">
+      <c r="AI2" s="24" t="s">
         <v>28</v>
       </c>
-      <c r="AJ2" s="25" t="s">
+      <c r="AJ2" s="24" t="s">
         <v>18</v>
       </c>
-      <c r="AK2" s="25" t="s">
+      <c r="AK2" s="24" t="s">
         <v>38</v>
       </c>
-      <c r="AL2" s="25" t="s">
+      <c r="AL2" s="24" t="s">
         <v>35</v>
       </c>
-      <c r="AM2" s="25" t="s">
+      <c r="AM2" s="24" t="s">
         <v>29</v>
       </c>
-      <c r="AN2" s="25" t="s">
+      <c r="AN2" s="24" t="s">
         <v>83</v>
       </c>
-      <c r="AO2" s="25" t="s">
+      <c r="AO2" s="24" t="s">
         <v>342</v>
       </c>
-      <c r="AP2" s="25" t="s">
+      <c r="AP2" s="24" t="s">
         <v>107</v>
       </c>
-      <c r="AQ2" s="25" t="s">
+      <c r="AQ2" s="24" t="s">
         <v>110</v>
       </c>
-      <c r="AR2" s="25" t="s">
+      <c r="AR2" s="24" t="s">
         <v>14</v>
       </c>
-      <c r="AS2" s="25" t="s">
+      <c r="AS2" s="24" t="s">
         <v>55</v>
       </c>
-      <c r="AT2" s="25" t="s">
+      <c r="AT2" s="24" t="s">
         <v>113</v>
       </c>
-      <c r="AU2" s="25" t="s">
+      <c r="AU2" s="24" t="s">
         <v>37</v>
       </c>
-      <c r="AV2" s="25" t="s">
+      <c r="AV2" s="24" t="s">
         <v>26</v>
       </c>
-      <c r="AW2" s="25" t="s">
+      <c r="AW2" s="24" t="s">
         <v>85</v>
       </c>
-      <c r="AX2" s="25" t="s">
+      <c r="AX2" s="24" t="s">
         <v>87</v>
       </c>
-      <c r="AY2" s="25" t="s">
+      <c r="AY2" s="24" t="s">
         <v>72</v>
       </c>
-      <c r="AZ2" s="25" t="s">
+      <c r="AZ2" s="24" t="s">
         <v>32</v>
       </c>
-      <c r="BA2" s="25" t="s">
+      <c r="BA2" s="24" t="s">
         <v>69</v>
       </c>
-      <c r="BB2" s="25" t="s">
+      <c r="BB2" s="24" t="s">
         <v>46</v>
       </c>
-      <c r="BC2" s="25" t="s">
+      <c r="BC2" s="24" t="s">
         <v>80</v>
       </c>
-      <c r="BD2" s="25" t="s">
+      <c r="BD2" s="24" t="s">
         <v>51</v>
       </c>
       <c r="BE2" s="19" t="s">
         <v>139</v>
       </c>
-      <c r="BF2" s="25" t="s">
+      <c r="BF2" s="24" t="s">
         <v>4</v>
       </c>
-      <c r="BG2" s="25" t="s">
+      <c r="BG2" s="24" t="s">
         <v>52</v>
       </c>
-      <c r="BH2" s="25" t="s">
+      <c r="BH2" s="24" t="s">
         <v>81</v>
       </c>
-      <c r="BI2" s="25" t="s">
+      <c r="BI2" s="24" t="s">
         <v>58</v>
       </c>
-      <c r="BJ2" s="25" t="s">
+      <c r="BJ2" s="24" t="s">
         <v>91</v>
       </c>
-      <c r="BK2" s="25" t="s">
+      <c r="BK2" s="24" t="s">
         <v>54</v>
       </c>
-      <c r="BL2" s="25" t="s">
+      <c r="BL2" s="24" t="s">
         <v>15</v>
       </c>
       <c r="BM2" s="17" t="s">
@@ -28184,115 +28434,115 @@
       <c r="BN2" s="19" t="s">
         <v>141</v>
       </c>
-      <c r="BO2" s="25" t="s">
+      <c r="BO2" s="24" t="s">
         <v>34</v>
       </c>
       <c r="BP2" s="19" t="s">
         <v>143</v>
       </c>
-      <c r="BQ2" s="25" t="s">
+      <c r="BQ2" s="24" t="s">
         <v>45</v>
       </c>
-      <c r="BR2" s="25" t="s">
+      <c r="BR2" s="24" t="s">
         <v>73</v>
       </c>
-      <c r="BS2" s="25" t="s">
-        <v>1</v>
-      </c>
-      <c r="BT2" s="25" t="s">
+      <c r="BS2" s="24" t="s">
+        <v>1</v>
+      </c>
+      <c r="BT2" s="24" t="s">
         <v>99</v>
       </c>
-      <c r="BU2" s="25" t="s">
+      <c r="BU2" s="24" t="s">
         <v>12</v>
       </c>
-      <c r="BV2" s="25" t="s">
+      <c r="BV2" s="24" t="s">
         <v>40</v>
       </c>
-      <c r="BW2" s="25" t="s">
+      <c r="BW2" s="24" t="s">
         <v>2</v>
       </c>
-      <c r="BX2" s="25" t="s">
+      <c r="BX2" s="24" t="s">
         <v>70</v>
       </c>
-      <c r="BY2" s="25" t="s">
+      <c r="BY2" s="24" t="s">
         <v>5</v>
       </c>
-      <c r="BZ2" s="25" t="s">
+      <c r="BZ2" s="24" t="s">
         <v>100</v>
       </c>
-      <c r="CA2" s="25" t="s">
+      <c r="CA2" s="24" t="s">
         <v>6</v>
       </c>
-      <c r="CB2" s="25" t="s">
+      <c r="CB2" s="24" t="s">
         <v>8</v>
       </c>
-      <c r="CC2" s="25" t="s">
+      <c r="CC2" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="CD2" s="25" t="s">
+      <c r="CD2" s="24" t="s">
         <v>21</v>
       </c>
-      <c r="CE2" s="25" t="s">
+      <c r="CE2" s="24" t="s">
         <v>96</v>
       </c>
-      <c r="CF2" s="25" t="s">
+      <c r="CF2" s="24" t="s">
         <v>9</v>
       </c>
-      <c r="CG2" s="25" t="s">
+      <c r="CG2" s="24" t="s">
         <v>7</v>
       </c>
       <c r="CH2" s="19" t="s">
         <v>349</v>
       </c>
-      <c r="CI2" s="25" t="s">
+      <c r="CI2" s="24" t="s">
         <v>20</v>
       </c>
-      <c r="CJ2" s="25" t="s">
+      <c r="CJ2" s="24" t="s">
         <v>36</v>
       </c>
-      <c r="CK2" s="25" t="s">
+      <c r="CK2" s="24" t="s">
         <v>13</v>
       </c>
-      <c r="CL2" s="25" t="s">
+      <c r="CL2" s="24" t="s">
         <v>19</v>
       </c>
-      <c r="CM2" s="25" t="s">
+      <c r="CM2" s="24" t="s">
         <v>17</v>
       </c>
-      <c r="CN2" s="25" t="s">
+      <c r="CN2" s="24" t="s">
         <v>30</v>
       </c>
-      <c r="CO2" s="25" t="s">
+      <c r="CO2" s="24" t="s">
         <v>44</v>
       </c>
-      <c r="CP2" s="25" t="s">
+      <c r="CP2" s="24" t="s">
         <v>60</v>
       </c>
-      <c r="CQ2" s="25" t="s">
+      <c r="CQ2" s="24" t="s">
         <v>57</v>
       </c>
-      <c r="CR2" s="25" t="s">
+      <c r="CR2" s="24" t="s">
         <v>27</v>
       </c>
       <c r="CS2" s="19" t="s">
         <v>146</v>
       </c>
-      <c r="CT2" s="25" t="s">
+      <c r="CT2" s="24" t="s">
         <v>59</v>
       </c>
-      <c r="CU2" s="25" t="s">
+      <c r="CU2" s="24" t="s">
         <v>25</v>
       </c>
-      <c r="CV2" s="25" t="s">
+      <c r="CV2" s="24" t="s">
         <v>88</v>
       </c>
-      <c r="CW2" s="25" t="s">
+      <c r="CW2" s="24" t="s">
         <v>68</v>
       </c>
       <c r="CX2" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="CY2" s="25" t="s">
+      <c r="CY2" s="24" t="s">
         <v>31</v>
       </c>
       <c r="CZ2" s="18" t="s">
@@ -28301,122 +28551,122 @@
     </row>
     <row r="3" spans="1:104" ht="87.6" x14ac:dyDescent="0.3">
       <c r="A3" s="17"/>
-      <c r="B3" s="25"/>
-      <c r="C3" s="25"/>
-      <c r="D3" s="25"/>
-      <c r="E3" s="25"/>
-      <c r="F3" s="25"/>
-      <c r="G3" s="25"/>
-      <c r="H3" s="25"/>
-      <c r="I3" s="25"/>
-      <c r="J3" s="25"/>
-      <c r="K3" s="25"/>
-      <c r="L3" s="25"/>
-      <c r="M3" s="25"/>
-      <c r="N3" s="25"/>
+      <c r="B3" s="24"/>
+      <c r="C3" s="24"/>
+      <c r="D3" s="24"/>
+      <c r="E3" s="24"/>
+      <c r="F3" s="24"/>
+      <c r="G3" s="24"/>
+      <c r="H3" s="24"/>
+      <c r="I3" s="24"/>
+      <c r="J3" s="24"/>
+      <c r="K3" s="24"/>
+      <c r="L3" s="24"/>
+      <c r="M3" s="24"/>
+      <c r="N3" s="24"/>
       <c r="O3" s="19" t="s">
         <v>133</v>
       </c>
       <c r="P3" s="19" t="s">
         <v>135</v>
       </c>
-      <c r="Q3" s="25"/>
-      <c r="R3" s="25"/>
-      <c r="S3" s="25"/>
-      <c r="T3" s="25"/>
-      <c r="U3" s="25"/>
-      <c r="V3" s="25"/>
-      <c r="W3" s="25"/>
-      <c r="X3" s="25"/>
-      <c r="Y3" s="25"/>
-      <c r="Z3" s="25"/>
+      <c r="Q3" s="24"/>
+      <c r="R3" s="24"/>
+      <c r="S3" s="24"/>
+      <c r="T3" s="24"/>
+      <c r="U3" s="24"/>
+      <c r="V3" s="24"/>
+      <c r="W3" s="24"/>
+      <c r="X3" s="24"/>
+      <c r="Y3" s="24"/>
+      <c r="Z3" s="24"/>
       <c r="AA3" s="17"/>
-      <c r="AB3" s="25"/>
-      <c r="AC3" s="25"/>
-      <c r="AD3" s="25"/>
-      <c r="AE3" s="25"/>
-      <c r="AF3" s="25"/>
-      <c r="AG3" s="25"/>
-      <c r="AH3" s="25"/>
-      <c r="AI3" s="25"/>
-      <c r="AJ3" s="25"/>
-      <c r="AK3" s="25"/>
-      <c r="AL3" s="25"/>
-      <c r="AM3" s="25"/>
-      <c r="AN3" s="25"/>
-      <c r="AO3" s="25"/>
-      <c r="AP3" s="25"/>
-      <c r="AQ3" s="25"/>
-      <c r="AR3" s="25"/>
-      <c r="AS3" s="25"/>
-      <c r="AT3" s="25"/>
-      <c r="AU3" s="25"/>
-      <c r="AV3" s="25"/>
-      <c r="AW3" s="25"/>
-      <c r="AX3" s="25"/>
-      <c r="AY3" s="25"/>
-      <c r="AZ3" s="25"/>
-      <c r="BA3" s="25"/>
-      <c r="BB3" s="25"/>
-      <c r="BC3" s="25"/>
-      <c r="BD3" s="25"/>
+      <c r="AB3" s="24"/>
+      <c r="AC3" s="24"/>
+      <c r="AD3" s="24"/>
+      <c r="AE3" s="24"/>
+      <c r="AF3" s="24"/>
+      <c r="AG3" s="24"/>
+      <c r="AH3" s="24"/>
+      <c r="AI3" s="24"/>
+      <c r="AJ3" s="24"/>
+      <c r="AK3" s="24"/>
+      <c r="AL3" s="24"/>
+      <c r="AM3" s="24"/>
+      <c r="AN3" s="24"/>
+      <c r="AO3" s="24"/>
+      <c r="AP3" s="24"/>
+      <c r="AQ3" s="24"/>
+      <c r="AR3" s="24"/>
+      <c r="AS3" s="24"/>
+      <c r="AT3" s="24"/>
+      <c r="AU3" s="24"/>
+      <c r="AV3" s="24"/>
+      <c r="AW3" s="24"/>
+      <c r="AX3" s="24"/>
+      <c r="AY3" s="24"/>
+      <c r="AZ3" s="24"/>
+      <c r="BA3" s="24"/>
+      <c r="BB3" s="24"/>
+      <c r="BC3" s="24"/>
+      <c r="BD3" s="24"/>
       <c r="BE3" s="19" t="s">
         <v>140</v>
       </c>
-      <c r="BF3" s="25"/>
-      <c r="BG3" s="25"/>
-      <c r="BH3" s="25"/>
-      <c r="BI3" s="25"/>
-      <c r="BJ3" s="25"/>
-      <c r="BK3" s="25"/>
-      <c r="BL3" s="25"/>
+      <c r="BF3" s="24"/>
+      <c r="BG3" s="24"/>
+      <c r="BH3" s="24"/>
+      <c r="BI3" s="24"/>
+      <c r="BJ3" s="24"/>
+      <c r="BK3" s="24"/>
+      <c r="BL3" s="24"/>
       <c r="BM3" s="17"/>
       <c r="BN3" s="19" t="s">
         <v>142</v>
       </c>
-      <c r="BO3" s="25"/>
+      <c r="BO3" s="24"/>
       <c r="BP3" s="19" t="s">
         <v>144</v>
       </c>
-      <c r="BQ3" s="25"/>
-      <c r="BR3" s="25"/>
-      <c r="BS3" s="25"/>
-      <c r="BT3" s="25"/>
-      <c r="BU3" s="25"/>
-      <c r="BV3" s="25"/>
-      <c r="BW3" s="25"/>
-      <c r="BX3" s="25"/>
-      <c r="BY3" s="25"/>
-      <c r="BZ3" s="25"/>
-      <c r="CA3" s="25"/>
-      <c r="CB3" s="25"/>
-      <c r="CC3" s="25"/>
-      <c r="CD3" s="25"/>
-      <c r="CE3" s="25"/>
-      <c r="CF3" s="25"/>
-      <c r="CG3" s="25"/>
+      <c r="BQ3" s="24"/>
+      <c r="BR3" s="24"/>
+      <c r="BS3" s="24"/>
+      <c r="BT3" s="24"/>
+      <c r="BU3" s="24"/>
+      <c r="BV3" s="24"/>
+      <c r="BW3" s="24"/>
+      <c r="BX3" s="24"/>
+      <c r="BY3" s="24"/>
+      <c r="BZ3" s="24"/>
+      <c r="CA3" s="24"/>
+      <c r="CB3" s="24"/>
+      <c r="CC3" s="24"/>
+      <c r="CD3" s="24"/>
+      <c r="CE3" s="24"/>
+      <c r="CF3" s="24"/>
+      <c r="CG3" s="24"/>
       <c r="CH3" s="19" t="s">
         <v>145</v>
       </c>
-      <c r="CI3" s="25"/>
-      <c r="CJ3" s="25"/>
-      <c r="CK3" s="25"/>
-      <c r="CL3" s="25"/>
-      <c r="CM3" s="25"/>
-      <c r="CN3" s="25"/>
-      <c r="CO3" s="25"/>
-      <c r="CP3" s="25"/>
-      <c r="CQ3" s="25"/>
-      <c r="CR3" s="25"/>
+      <c r="CI3" s="24"/>
+      <c r="CJ3" s="24"/>
+      <c r="CK3" s="24"/>
+      <c r="CL3" s="24"/>
+      <c r="CM3" s="24"/>
+      <c r="CN3" s="24"/>
+      <c r="CO3" s="24"/>
+      <c r="CP3" s="24"/>
+      <c r="CQ3" s="24"/>
+      <c r="CR3" s="24"/>
       <c r="CS3" s="19" t="s">
         <v>133</v>
       </c>
-      <c r="CT3" s="25"/>
-      <c r="CU3" s="25"/>
-      <c r="CV3" s="25"/>
-      <c r="CW3" s="25"/>
+      <c r="CT3" s="24"/>
+      <c r="CU3" s="24"/>
+      <c r="CV3" s="24"/>
+      <c r="CW3" s="24"/>
       <c r="CX3" s="19"/>
-      <c r="CY3" s="25"/>
+      <c r="CY3" s="24"/>
       <c r="CZ3" s="18"/>
     </row>
     <row r="4" spans="1:104" x14ac:dyDescent="0.3">
@@ -37134,88 +37384,6 @@
     </row>
   </sheetData>
   <mergeCells count="106">
-    <mergeCell ref="CR2:CR3"/>
-    <mergeCell ref="CT2:CT3"/>
-    <mergeCell ref="CU2:CU3"/>
-    <mergeCell ref="CV2:CV3"/>
-    <mergeCell ref="CW2:CW3"/>
-    <mergeCell ref="CY2:CY3"/>
-    <mergeCell ref="CL2:CL3"/>
-    <mergeCell ref="CM2:CM3"/>
-    <mergeCell ref="CN2:CN3"/>
-    <mergeCell ref="CO2:CO3"/>
-    <mergeCell ref="CP2:CP3"/>
-    <mergeCell ref="CQ2:CQ3"/>
-    <mergeCell ref="CE2:CE3"/>
-    <mergeCell ref="CF2:CF3"/>
-    <mergeCell ref="CG2:CG3"/>
-    <mergeCell ref="CI2:CI3"/>
-    <mergeCell ref="CJ2:CJ3"/>
-    <mergeCell ref="CK2:CK3"/>
-    <mergeCell ref="BY2:BY3"/>
-    <mergeCell ref="BZ2:BZ3"/>
-    <mergeCell ref="CA2:CA3"/>
-    <mergeCell ref="CB2:CB3"/>
-    <mergeCell ref="CC2:CC3"/>
-    <mergeCell ref="CD2:CD3"/>
-    <mergeCell ref="BS2:BS3"/>
-    <mergeCell ref="BT2:BT3"/>
-    <mergeCell ref="BU2:BU3"/>
-    <mergeCell ref="BV2:BV3"/>
-    <mergeCell ref="BW2:BW3"/>
-    <mergeCell ref="BX2:BX3"/>
-    <mergeCell ref="BJ2:BJ3"/>
-    <mergeCell ref="BK2:BK3"/>
-    <mergeCell ref="BL2:BL3"/>
-    <mergeCell ref="BO2:BO3"/>
-    <mergeCell ref="BQ2:BQ3"/>
-    <mergeCell ref="BR2:BR3"/>
-    <mergeCell ref="BC2:BC3"/>
-    <mergeCell ref="BD2:BD3"/>
-    <mergeCell ref="BF2:BF3"/>
-    <mergeCell ref="BG2:BG3"/>
-    <mergeCell ref="BH2:BH3"/>
-    <mergeCell ref="BI2:BI3"/>
-    <mergeCell ref="AW2:AW3"/>
-    <mergeCell ref="AX2:AX3"/>
-    <mergeCell ref="AY2:AY3"/>
-    <mergeCell ref="AZ2:AZ3"/>
-    <mergeCell ref="BA2:BA3"/>
-    <mergeCell ref="BB2:BB3"/>
-    <mergeCell ref="AQ2:AQ3"/>
-    <mergeCell ref="AR2:AR3"/>
-    <mergeCell ref="AS2:AS3"/>
-    <mergeCell ref="AT2:AT3"/>
-    <mergeCell ref="AU2:AU3"/>
-    <mergeCell ref="AV2:AV3"/>
-    <mergeCell ref="AK2:AK3"/>
-    <mergeCell ref="AL2:AL3"/>
-    <mergeCell ref="AM2:AM3"/>
-    <mergeCell ref="AN2:AN3"/>
-    <mergeCell ref="AO2:AO3"/>
-    <mergeCell ref="AP2:AP3"/>
-    <mergeCell ref="AE2:AE3"/>
-    <mergeCell ref="AF2:AF3"/>
-    <mergeCell ref="AG2:AG3"/>
-    <mergeCell ref="AH2:AH3"/>
-    <mergeCell ref="AI2:AI3"/>
-    <mergeCell ref="AJ2:AJ3"/>
-    <mergeCell ref="X2:X3"/>
-    <mergeCell ref="Y2:Y3"/>
-    <mergeCell ref="Z2:Z3"/>
-    <mergeCell ref="AB2:AB3"/>
-    <mergeCell ref="AC2:AC3"/>
-    <mergeCell ref="AD2:AD3"/>
-    <mergeCell ref="T2:T3"/>
-    <mergeCell ref="U2:U3"/>
-    <mergeCell ref="V2:V3"/>
-    <mergeCell ref="W2:W3"/>
-    <mergeCell ref="J2:J3"/>
-    <mergeCell ref="K2:K3"/>
-    <mergeCell ref="L2:L3"/>
-    <mergeCell ref="M2:M3"/>
-    <mergeCell ref="N2:N3"/>
-    <mergeCell ref="Q2:Q3"/>
     <mergeCell ref="CH1:CQ1"/>
     <mergeCell ref="CR1:CY1"/>
     <mergeCell ref="B2:B3"/>
@@ -37240,6 +37408,88 @@
     <mergeCell ref="AB1:AF1"/>
     <mergeCell ref="R2:R3"/>
     <mergeCell ref="S2:S3"/>
+    <mergeCell ref="T2:T3"/>
+    <mergeCell ref="U2:U3"/>
+    <mergeCell ref="V2:V3"/>
+    <mergeCell ref="W2:W3"/>
+    <mergeCell ref="J2:J3"/>
+    <mergeCell ref="K2:K3"/>
+    <mergeCell ref="L2:L3"/>
+    <mergeCell ref="M2:M3"/>
+    <mergeCell ref="N2:N3"/>
+    <mergeCell ref="Q2:Q3"/>
+    <mergeCell ref="AE2:AE3"/>
+    <mergeCell ref="AF2:AF3"/>
+    <mergeCell ref="AG2:AG3"/>
+    <mergeCell ref="AH2:AH3"/>
+    <mergeCell ref="AI2:AI3"/>
+    <mergeCell ref="AJ2:AJ3"/>
+    <mergeCell ref="X2:X3"/>
+    <mergeCell ref="Y2:Y3"/>
+    <mergeCell ref="Z2:Z3"/>
+    <mergeCell ref="AB2:AB3"/>
+    <mergeCell ref="AC2:AC3"/>
+    <mergeCell ref="AD2:AD3"/>
+    <mergeCell ref="AQ2:AQ3"/>
+    <mergeCell ref="AR2:AR3"/>
+    <mergeCell ref="AS2:AS3"/>
+    <mergeCell ref="AT2:AT3"/>
+    <mergeCell ref="AU2:AU3"/>
+    <mergeCell ref="AV2:AV3"/>
+    <mergeCell ref="AK2:AK3"/>
+    <mergeCell ref="AL2:AL3"/>
+    <mergeCell ref="AM2:AM3"/>
+    <mergeCell ref="AN2:AN3"/>
+    <mergeCell ref="AO2:AO3"/>
+    <mergeCell ref="AP2:AP3"/>
+    <mergeCell ref="BC2:BC3"/>
+    <mergeCell ref="BD2:BD3"/>
+    <mergeCell ref="BF2:BF3"/>
+    <mergeCell ref="BG2:BG3"/>
+    <mergeCell ref="BH2:BH3"/>
+    <mergeCell ref="BI2:BI3"/>
+    <mergeCell ref="AW2:AW3"/>
+    <mergeCell ref="AX2:AX3"/>
+    <mergeCell ref="AY2:AY3"/>
+    <mergeCell ref="AZ2:AZ3"/>
+    <mergeCell ref="BA2:BA3"/>
+    <mergeCell ref="BB2:BB3"/>
+    <mergeCell ref="BS2:BS3"/>
+    <mergeCell ref="BT2:BT3"/>
+    <mergeCell ref="BU2:BU3"/>
+    <mergeCell ref="BV2:BV3"/>
+    <mergeCell ref="BW2:BW3"/>
+    <mergeCell ref="BX2:BX3"/>
+    <mergeCell ref="BJ2:BJ3"/>
+    <mergeCell ref="BK2:BK3"/>
+    <mergeCell ref="BL2:BL3"/>
+    <mergeCell ref="BO2:BO3"/>
+    <mergeCell ref="BQ2:BQ3"/>
+    <mergeCell ref="BR2:BR3"/>
+    <mergeCell ref="CE2:CE3"/>
+    <mergeCell ref="CF2:CF3"/>
+    <mergeCell ref="CG2:CG3"/>
+    <mergeCell ref="CI2:CI3"/>
+    <mergeCell ref="CJ2:CJ3"/>
+    <mergeCell ref="CK2:CK3"/>
+    <mergeCell ref="BY2:BY3"/>
+    <mergeCell ref="BZ2:BZ3"/>
+    <mergeCell ref="CA2:CA3"/>
+    <mergeCell ref="CB2:CB3"/>
+    <mergeCell ref="CC2:CC3"/>
+    <mergeCell ref="CD2:CD3"/>
+    <mergeCell ref="CR2:CR3"/>
+    <mergeCell ref="CT2:CT3"/>
+    <mergeCell ref="CU2:CU3"/>
+    <mergeCell ref="CV2:CV3"/>
+    <mergeCell ref="CW2:CW3"/>
+    <mergeCell ref="CY2:CY3"/>
+    <mergeCell ref="CL2:CL3"/>
+    <mergeCell ref="CM2:CM3"/>
+    <mergeCell ref="CN2:CN3"/>
+    <mergeCell ref="CO2:CO3"/>
+    <mergeCell ref="CP2:CP3"/>
+    <mergeCell ref="CQ2:CQ3"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1" tooltip="2020 coronavirus pandemic in Argentina" display="https://en.wikipedia.org/wiki/2020_coronavirus_pandemic_in_Argentina" xr:uid="{A1276897-A83E-4B5D-8DEB-71FFBF97F299}"/>

</xml_diff>